<commit_message>
new mapping & front-end bug fix
</commit_message>
<xml_diff>
--- a/server/excel_mapping/GDC CTCAE v5.0 Map 2018.05.02.xlsx
+++ b/server/excel_mapping/GDC CTCAE v5.0 Map 2018.05.02.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patelbhp\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patelbhp\Desktop\GDCMVS\server\excel_mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,10 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="GDC CTCAE v5.0" sheetId="1" r:id="rId1"/>
-    <sheet name="Deprecated in v5.0" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Deprecated in v5.0'!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'GDC CTCAE v5.0'!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
@@ -29,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4726" uniqueCount="2355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4674" uniqueCount="2343">
   <si>
     <t>Category</t>
   </si>
@@ -7058,42 +7056,6 @@
   </si>
   <si>
     <t>C58404</t>
-  </si>
-  <si>
-    <t>Acute Coronary Syndrome</t>
-  </si>
-  <si>
-    <t>Constrictive Pericarditis</t>
-  </si>
-  <si>
-    <t>External Ear Inflammation</t>
-  </si>
-  <si>
-    <t>Fallopian Tube Stenosis</t>
-  </si>
-  <si>
-    <t>Female Genital Tract Fistula</t>
-  </si>
-  <si>
-    <t>Fetal Death</t>
-  </si>
-  <si>
-    <t>Intraoperative Skin Injury</t>
-  </si>
-  <si>
-    <t>Menopause</t>
-  </si>
-  <si>
-    <t>Spleen Disorder</t>
-  </si>
-  <si>
-    <t>Unintended Pregnancy</t>
-  </si>
-  <si>
-    <t>Vaginismus</t>
-  </si>
-  <si>
-    <t>Wolff-Parkinson-White Syndrome</t>
   </si>
 </sst>
 </file>
@@ -7178,10 +7140,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7202,37 +7163,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="43">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -7976,7 +7907,7 @@
   <dimension ref="A1:F1354"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.69140625" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -7986,26 +7917,26 @@
     <col min="4" max="4" width="41" style="1" customWidth="1"/>
     <col min="5" max="5" width="42.69140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.69140625" style="1"/>
-    <col min="7" max="16384" width="11.69140625" style="3"/>
+    <col min="7" max="16384" width="11.69140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -19099,7 +19030,7 @@
       <c r="C556" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D556" s="4" t="s">
+      <c r="D556" s="3" t="s">
         <v>1263</v>
       </c>
       <c r="E556" s="1" t="s">
@@ -22650,7 +22581,7 @@
       </c>
     </row>
     <row r="734" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A734" s="4" t="s">
+      <c r="A734" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B734" s="1" t="s">
@@ -22670,7 +22601,7 @@
       </c>
     </row>
     <row r="735" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A735" s="4" t="s">
+      <c r="A735" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B735" s="1" t="s">
@@ -22690,7 +22621,7 @@
       </c>
     </row>
     <row r="736" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A736" s="4" t="s">
+      <c r="A736" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B736" s="1" t="s">
@@ -22710,7 +22641,7 @@
       </c>
     </row>
     <row r="737" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A737" s="4" t="s">
+      <c r="A737" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B737" s="1" t="s">
@@ -22730,7 +22661,7 @@
       </c>
     </row>
     <row r="738" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A738" s="4" t="s">
+      <c r="A738" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B738" s="1" t="s">
@@ -22750,7 +22681,7 @@
       </c>
     </row>
     <row r="739" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A739" s="4" t="s">
+      <c r="A739" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B739" s="1" t="s">
@@ -22770,7 +22701,7 @@
       </c>
     </row>
     <row r="740" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A740" s="4" t="s">
+      <c r="A740" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B740" s="1" t="s">
@@ -22790,7 +22721,7 @@
       </c>
     </row>
     <row r="741" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A741" s="4" t="s">
+      <c r="A741" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B741" s="1" t="s">
@@ -22810,7 +22741,7 @@
       </c>
     </row>
     <row r="742" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A742" s="4" t="s">
+      <c r="A742" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B742" s="1" t="s">
@@ -22830,7 +22761,7 @@
       </c>
     </row>
     <row r="743" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A743" s="4" t="s">
+      <c r="A743" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B743" s="1" t="s">
@@ -22850,7 +22781,7 @@
       </c>
     </row>
     <row r="744" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A744" s="4" t="s">
+      <c r="A744" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B744" s="1" t="s">
@@ -22870,7 +22801,7 @@
       </c>
     </row>
     <row r="745" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A745" s="4" t="s">
+      <c r="A745" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B745" s="1" t="s">
@@ -22890,7 +22821,7 @@
       </c>
     </row>
     <row r="746" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A746" s="4" t="s">
+      <c r="A746" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B746" s="1" t="s">
@@ -22910,7 +22841,7 @@
       </c>
     </row>
     <row r="747" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A747" s="4" t="s">
+      <c r="A747" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B747" s="1" t="s">
@@ -22930,7 +22861,7 @@
       </c>
     </row>
     <row r="748" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A748" s="4" t="s">
+      <c r="A748" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B748" s="1" t="s">
@@ -22950,7 +22881,7 @@
       </c>
     </row>
     <row r="749" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A749" s="4" t="s">
+      <c r="A749" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B749" s="1" t="s">
@@ -22970,7 +22901,7 @@
       </c>
     </row>
     <row r="750" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A750" s="4" t="s">
+      <c r="A750" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B750" s="1" t="s">
@@ -22990,7 +22921,7 @@
       </c>
     </row>
     <row r="751" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A751" s="4" t="s">
+      <c r="A751" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B751" s="1" t="s">
@@ -23010,7 +22941,7 @@
       </c>
     </row>
     <row r="752" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A752" s="4" t="s">
+      <c r="A752" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B752" s="1" t="s">
@@ -23030,7 +22961,7 @@
       </c>
     </row>
     <row r="753" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A753" s="4" t="s">
+      <c r="A753" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B753" s="1" t="s">
@@ -23050,7 +22981,7 @@
       </c>
     </row>
     <row r="754" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A754" s="4" t="s">
+      <c r="A754" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B754" s="1" t="s">
@@ -23070,7 +23001,7 @@
       </c>
     </row>
     <row r="755" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A755" s="4" t="s">
+      <c r="A755" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B755" s="1" t="s">
@@ -23090,7 +23021,7 @@
       </c>
     </row>
     <row r="756" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A756" s="4" t="s">
+      <c r="A756" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B756" s="1" t="s">
@@ -23110,7 +23041,7 @@
       </c>
     </row>
     <row r="757" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A757" s="4" t="s">
+      <c r="A757" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B757" s="1" t="s">
@@ -23130,7 +23061,7 @@
       </c>
     </row>
     <row r="758" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A758" s="4" t="s">
+      <c r="A758" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B758" s="1" t="s">
@@ -23150,7 +23081,7 @@
       </c>
     </row>
     <row r="759" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A759" s="4" t="s">
+      <c r="A759" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B759" s="1" t="s">
@@ -23170,7 +23101,7 @@
       </c>
     </row>
     <row r="760" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A760" s="4" t="s">
+      <c r="A760" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B760" s="1" t="s">
@@ -23190,7 +23121,7 @@
       </c>
     </row>
     <row r="761" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A761" s="4" t="s">
+      <c r="A761" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B761" s="1" t="s">
@@ -23210,7 +23141,7 @@
       </c>
     </row>
     <row r="762" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A762" s="4" t="s">
+      <c r="A762" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B762" s="1" t="s">
@@ -23230,7 +23161,7 @@
       </c>
     </row>
     <row r="763" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A763" s="4" t="s">
+      <c r="A763" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B763" s="1" t="s">
@@ -23250,7 +23181,7 @@
       </c>
     </row>
     <row r="764" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A764" s="4" t="s">
+      <c r="A764" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B764" s="1" t="s">
@@ -23270,7 +23201,7 @@
       </c>
     </row>
     <row r="765" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A765" s="4" t="s">
+      <c r="A765" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B765" s="1" t="s">
@@ -23290,7 +23221,7 @@
       </c>
     </row>
     <row r="766" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A766" s="4" t="s">
+      <c r="A766" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B766" s="1" t="s">
@@ -23310,7 +23241,7 @@
       </c>
     </row>
     <row r="767" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A767" s="4" t="s">
+      <c r="A767" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B767" s="1" t="s">
@@ -23330,7 +23261,7 @@
       </c>
     </row>
     <row r="768" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A768" s="4" t="s">
+      <c r="A768" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B768" s="1" t="s">
@@ -23350,7 +23281,7 @@
       </c>
     </row>
     <row r="769" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A769" s="4" t="s">
+      <c r="A769" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B769" s="1" t="s">
@@ -23370,7 +23301,7 @@
       </c>
     </row>
     <row r="770" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A770" s="4" t="s">
+      <c r="A770" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B770" s="1" t="s">
@@ -23390,7 +23321,7 @@
       </c>
     </row>
     <row r="771" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A771" s="4" t="s">
+      <c r="A771" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B771" s="1" t="s">
@@ -23410,7 +23341,7 @@
       </c>
     </row>
     <row r="772" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A772" s="4" t="s">
+      <c r="A772" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B772" s="1" t="s">
@@ -23430,7 +23361,7 @@
       </c>
     </row>
     <row r="773" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A773" s="4" t="s">
+      <c r="A773" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B773" s="1" t="s">
@@ -23450,7 +23381,7 @@
       </c>
     </row>
     <row r="774" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A774" s="4" t="s">
+      <c r="A774" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B774" s="1" t="s">
@@ -23470,7 +23401,7 @@
       </c>
     </row>
     <row r="775" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A775" s="4" t="s">
+      <c r="A775" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B775" s="1" t="s">
@@ -23490,7 +23421,7 @@
       </c>
     </row>
     <row r="776" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A776" s="4" t="s">
+      <c r="A776" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B776" s="1" t="s">
@@ -23510,7 +23441,7 @@
       </c>
     </row>
     <row r="777" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A777" s="4" t="s">
+      <c r="A777" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B777" s="1" t="s">
@@ -23530,7 +23461,7 @@
       </c>
     </row>
     <row r="778" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A778" s="4" t="s">
+      <c r="A778" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B778" s="1" t="s">
@@ -23550,7 +23481,7 @@
       </c>
     </row>
     <row r="779" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A779" s="4" t="s">
+      <c r="A779" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B779" s="1" t="s">
@@ -23570,2292 +23501,2292 @@
       </c>
     </row>
     <row r="780" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A780" s="4"/>
+      <c r="A780" s="3"/>
     </row>
     <row r="781" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A781" s="4"/>
+      <c r="A781" s="3"/>
     </row>
     <row r="782" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A782" s="4"/>
+      <c r="A782" s="3"/>
     </row>
     <row r="783" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A783" s="4"/>
+      <c r="A783" s="3"/>
     </row>
     <row r="784" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A784" s="4"/>
+      <c r="A784" s="3"/>
     </row>
     <row r="785" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A785" s="4"/>
+      <c r="A785" s="3"/>
     </row>
     <row r="786" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A786" s="4"/>
+      <c r="A786" s="3"/>
     </row>
     <row r="787" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A787" s="4"/>
+      <c r="A787" s="3"/>
     </row>
     <row r="788" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A788" s="4"/>
+      <c r="A788" s="3"/>
     </row>
     <row r="789" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A789" s="4"/>
+      <c r="A789" s="3"/>
     </row>
     <row r="790" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A790" s="4"/>
+      <c r="A790" s="3"/>
     </row>
     <row r="791" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A791" s="4"/>
+      <c r="A791" s="3"/>
     </row>
     <row r="792" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A792" s="5"/>
-      <c r="B792" s="6"/>
+      <c r="A792" s="4"/>
+      <c r="B792" s="5"/>
     </row>
     <row r="793" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A793" s="5"/>
-      <c r="B793" s="6"/>
+      <c r="A793" s="4"/>
+      <c r="B793" s="5"/>
     </row>
     <row r="794" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A794" s="5"/>
-      <c r="B794" s="6"/>
+      <c r="A794" s="4"/>
+      <c r="B794" s="5"/>
     </row>
     <row r="795" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A795" s="5"/>
-      <c r="B795" s="6"/>
+      <c r="A795" s="4"/>
+      <c r="B795" s="5"/>
     </row>
     <row r="796" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A796" s="5"/>
-      <c r="B796" s="6"/>
+      <c r="A796" s="4"/>
+      <c r="B796" s="5"/>
     </row>
     <row r="797" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A797" s="5"/>
-      <c r="B797" s="6"/>
+      <c r="A797" s="4"/>
+      <c r="B797" s="5"/>
     </row>
     <row r="798" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A798" s="5"/>
-      <c r="B798" s="6"/>
+      <c r="A798" s="4"/>
+      <c r="B798" s="5"/>
     </row>
     <row r="799" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A799" s="5"/>
-      <c r="B799" s="6"/>
+      <c r="A799" s="4"/>
+      <c r="B799" s="5"/>
     </row>
     <row r="800" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A800" s="5"/>
-      <c r="B800" s="6"/>
+      <c r="A800" s="4"/>
+      <c r="B800" s="5"/>
     </row>
     <row r="801" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A801" s="5"/>
-      <c r="B801" s="6"/>
+      <c r="A801" s="4"/>
+      <c r="B801" s="5"/>
     </row>
     <row r="802" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A802" s="5"/>
-      <c r="B802" s="6"/>
+      <c r="A802" s="4"/>
+      <c r="B802" s="5"/>
     </row>
     <row r="803" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A803" s="5"/>
-      <c r="B803" s="6"/>
+      <c r="A803" s="4"/>
+      <c r="B803" s="5"/>
     </row>
     <row r="804" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A804" s="5"/>
-      <c r="B804" s="6"/>
+      <c r="A804" s="4"/>
+      <c r="B804" s="5"/>
     </row>
     <row r="805" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A805" s="5"/>
-      <c r="B805" s="6"/>
+      <c r="A805" s="4"/>
+      <c r="B805" s="5"/>
     </row>
     <row r="806" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A806" s="5"/>
-      <c r="B806" s="6"/>
+      <c r="A806" s="4"/>
+      <c r="B806" s="5"/>
     </row>
     <row r="807" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A807" s="5"/>
-      <c r="B807" s="6"/>
+      <c r="A807" s="4"/>
+      <c r="B807" s="5"/>
     </row>
     <row r="808" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A808" s="5"/>
-      <c r="B808" s="6"/>
+      <c r="A808" s="4"/>
+      <c r="B808" s="5"/>
     </row>
     <row r="809" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A809" s="5"/>
-      <c r="B809" s="6"/>
+      <c r="A809" s="4"/>
+      <c r="B809" s="5"/>
     </row>
     <row r="810" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A810" s="7"/>
-      <c r="B810" s="6"/>
+      <c r="A810" s="6"/>
+      <c r="B810" s="5"/>
     </row>
     <row r="811" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A811" s="7"/>
-      <c r="B811" s="6"/>
+      <c r="A811" s="6"/>
+      <c r="B811" s="5"/>
     </row>
     <row r="812" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A812" s="7"/>
-      <c r="B812" s="6"/>
+      <c r="A812" s="6"/>
+      <c r="B812" s="5"/>
     </row>
     <row r="813" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A813" s="7"/>
-      <c r="B813" s="6"/>
+      <c r="A813" s="6"/>
+      <c r="B813" s="5"/>
     </row>
     <row r="814" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A814" s="7"/>
-      <c r="B814" s="6"/>
+      <c r="A814" s="6"/>
+      <c r="B814" s="5"/>
     </row>
     <row r="815" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A815" s="7"/>
-      <c r="B815" s="6"/>
+      <c r="A815" s="6"/>
+      <c r="B815" s="5"/>
     </row>
     <row r="816" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A816" s="7"/>
-      <c r="B816" s="6"/>
+      <c r="A816" s="6"/>
+      <c r="B816" s="5"/>
     </row>
     <row r="817" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A817" s="7"/>
-      <c r="B817" s="6"/>
+      <c r="A817" s="6"/>
+      <c r="B817" s="5"/>
     </row>
     <row r="818" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A818" s="7"/>
-      <c r="B818" s="6"/>
+      <c r="A818" s="6"/>
+      <c r="B818" s="5"/>
     </row>
     <row r="819" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A819" s="7"/>
-      <c r="B819" s="6"/>
+      <c r="A819" s="6"/>
+      <c r="B819" s="5"/>
     </row>
     <row r="820" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A820" s="7"/>
-      <c r="B820" s="6"/>
+      <c r="A820" s="6"/>
+      <c r="B820" s="5"/>
     </row>
     <row r="821" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A821" s="7"/>
-      <c r="B821" s="6"/>
+      <c r="A821" s="6"/>
+      <c r="B821" s="5"/>
     </row>
     <row r="822" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A822" s="7"/>
-      <c r="B822" s="6"/>
+      <c r="A822" s="6"/>
+      <c r="B822" s="5"/>
     </row>
     <row r="823" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A823" s="7"/>
-      <c r="B823" s="6"/>
+      <c r="A823" s="6"/>
+      <c r="B823" s="5"/>
     </row>
     <row r="824" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A824" s="7"/>
-      <c r="B824" s="6"/>
+      <c r="A824" s="6"/>
+      <c r="B824" s="5"/>
     </row>
     <row r="825" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A825" s="7"/>
-      <c r="B825" s="6"/>
+      <c r="A825" s="6"/>
+      <c r="B825" s="5"/>
     </row>
     <row r="826" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A826" s="7"/>
-      <c r="B826" s="6"/>
+      <c r="A826" s="6"/>
+      <c r="B826" s="5"/>
     </row>
     <row r="827" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A827" s="7"/>
-      <c r="B827" s="6"/>
+      <c r="A827" s="6"/>
+      <c r="B827" s="5"/>
     </row>
     <row r="828" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A828" s="7"/>
-      <c r="B828" s="6"/>
+      <c r="A828" s="6"/>
+      <c r="B828" s="5"/>
     </row>
     <row r="829" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A829" s="7"/>
-      <c r="B829" s="6"/>
+      <c r="A829" s="6"/>
+      <c r="B829" s="5"/>
     </row>
     <row r="830" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A830" s="7"/>
-      <c r="B830" s="6"/>
+      <c r="A830" s="6"/>
+      <c r="B830" s="5"/>
     </row>
     <row r="831" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A831" s="7"/>
-      <c r="B831" s="6"/>
+      <c r="A831" s="6"/>
+      <c r="B831" s="5"/>
     </row>
     <row r="832" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A832" s="7"/>
-      <c r="B832" s="6"/>
+      <c r="A832" s="6"/>
+      <c r="B832" s="5"/>
     </row>
     <row r="833" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A833" s="7"/>
-      <c r="B833" s="6"/>
+      <c r="A833" s="6"/>
+      <c r="B833" s="5"/>
     </row>
     <row r="834" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A834" s="7"/>
-      <c r="B834" s="6"/>
+      <c r="A834" s="6"/>
+      <c r="B834" s="5"/>
     </row>
     <row r="835" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A835" s="7"/>
-      <c r="B835" s="6"/>
+      <c r="A835" s="6"/>
+      <c r="B835" s="5"/>
     </row>
     <row r="836" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A836" s="7"/>
-      <c r="B836" s="6"/>
+      <c r="A836" s="6"/>
+      <c r="B836" s="5"/>
     </row>
     <row r="837" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A837" s="7"/>
-      <c r="B837" s="6"/>
+      <c r="A837" s="6"/>
+      <c r="B837" s="5"/>
     </row>
     <row r="838" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A838" s="5"/>
-      <c r="B838" s="6"/>
+      <c r="A838" s="4"/>
+      <c r="B838" s="5"/>
     </row>
     <row r="839" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A839" s="7"/>
-      <c r="B839" s="6"/>
+      <c r="A839" s="6"/>
+      <c r="B839" s="5"/>
     </row>
     <row r="840" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A840" s="7"/>
-      <c r="B840" s="6"/>
+      <c r="A840" s="6"/>
+      <c r="B840" s="5"/>
     </row>
     <row r="841" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A841" s="7"/>
-      <c r="B841" s="6"/>
+      <c r="A841" s="6"/>
+      <c r="B841" s="5"/>
     </row>
     <row r="842" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A842" s="7"/>
-      <c r="B842" s="6"/>
+      <c r="A842" s="6"/>
+      <c r="B842" s="5"/>
     </row>
     <row r="843" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A843" s="7"/>
-      <c r="B843" s="6"/>
+      <c r="A843" s="6"/>
+      <c r="B843" s="5"/>
     </row>
     <row r="844" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A844" s="7"/>
-      <c r="B844" s="6"/>
+      <c r="A844" s="6"/>
+      <c r="B844" s="5"/>
     </row>
     <row r="845" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A845" s="7"/>
-      <c r="B845" s="6"/>
+      <c r="A845" s="6"/>
+      <c r="B845" s="5"/>
     </row>
     <row r="846" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A846" s="7"/>
-      <c r="B846" s="6"/>
+      <c r="A846" s="6"/>
+      <c r="B846" s="5"/>
     </row>
     <row r="847" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A847" s="7"/>
-      <c r="B847" s="6"/>
+      <c r="A847" s="6"/>
+      <c r="B847" s="5"/>
     </row>
     <row r="848" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A848" s="7"/>
-      <c r="B848" s="6"/>
+      <c r="A848" s="6"/>
+      <c r="B848" s="5"/>
     </row>
     <row r="849" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A849" s="7"/>
-      <c r="B849" s="6"/>
+      <c r="A849" s="6"/>
+      <c r="B849" s="5"/>
     </row>
     <row r="850" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A850" s="7"/>
-      <c r="B850" s="6"/>
+      <c r="A850" s="6"/>
+      <c r="B850" s="5"/>
     </row>
     <row r="851" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A851" s="7"/>
-      <c r="B851" s="6"/>
+      <c r="A851" s="6"/>
+      <c r="B851" s="5"/>
     </row>
     <row r="852" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A852" s="7"/>
-      <c r="B852" s="6"/>
+      <c r="A852" s="6"/>
+      <c r="B852" s="5"/>
     </row>
     <row r="853" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A853" s="7"/>
-      <c r="B853" s="6"/>
+      <c r="A853" s="6"/>
+      <c r="B853" s="5"/>
     </row>
     <row r="854" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A854" s="7"/>
-      <c r="B854" s="6"/>
+      <c r="A854" s="6"/>
+      <c r="B854" s="5"/>
     </row>
     <row r="855" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A855" s="5"/>
-      <c r="B855" s="6"/>
+      <c r="A855" s="4"/>
+      <c r="B855" s="5"/>
     </row>
     <row r="856" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A856" s="5"/>
-      <c r="B856" s="6"/>
+      <c r="A856" s="4"/>
+      <c r="B856" s="5"/>
     </row>
     <row r="857" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A857" s="5"/>
-      <c r="B857" s="6"/>
+      <c r="A857" s="4"/>
+      <c r="B857" s="5"/>
     </row>
     <row r="858" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A858" s="5"/>
-      <c r="B858" s="6"/>
+      <c r="A858" s="4"/>
+      <c r="B858" s="5"/>
     </row>
     <row r="859" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A859" s="5"/>
-      <c r="B859" s="6"/>
+      <c r="A859" s="4"/>
+      <c r="B859" s="5"/>
     </row>
     <row r="860" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A860" s="5"/>
-      <c r="B860" s="6"/>
+      <c r="A860" s="4"/>
+      <c r="B860" s="5"/>
     </row>
     <row r="861" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A861" s="5"/>
-      <c r="B861" s="6"/>
+      <c r="A861" s="4"/>
+      <c r="B861" s="5"/>
     </row>
     <row r="862" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A862" s="5"/>
-      <c r="B862" s="6"/>
+      <c r="A862" s="4"/>
+      <c r="B862" s="5"/>
     </row>
     <row r="863" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A863" s="5"/>
-      <c r="B863" s="6"/>
+      <c r="A863" s="4"/>
+      <c r="B863" s="5"/>
     </row>
     <row r="864" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A864" s="5"/>
-      <c r="B864" s="6"/>
+      <c r="A864" s="4"/>
+      <c r="B864" s="5"/>
     </row>
     <row r="865" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A865" s="5"/>
-      <c r="B865" s="6"/>
+      <c r="A865" s="4"/>
+      <c r="B865" s="5"/>
     </row>
     <row r="866" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A866" s="5"/>
-      <c r="B866" s="6"/>
+      <c r="A866" s="4"/>
+      <c r="B866" s="5"/>
     </row>
     <row r="867" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A867" s="5"/>
-      <c r="B867" s="6"/>
+      <c r="A867" s="4"/>
+      <c r="B867" s="5"/>
     </row>
     <row r="868" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A868" s="5"/>
-      <c r="B868" s="6"/>
+      <c r="A868" s="4"/>
+      <c r="B868" s="5"/>
     </row>
     <row r="869" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A869" s="5"/>
-      <c r="B869" s="6"/>
+      <c r="A869" s="4"/>
+      <c r="B869" s="5"/>
     </row>
     <row r="870" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A870" s="5"/>
-      <c r="B870" s="6"/>
+      <c r="A870" s="4"/>
+      <c r="B870" s="5"/>
     </row>
     <row r="871" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A871" s="5"/>
-      <c r="B871" s="6"/>
+      <c r="A871" s="4"/>
+      <c r="B871" s="5"/>
     </row>
     <row r="872" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A872" s="5"/>
-      <c r="B872" s="6"/>
+      <c r="A872" s="4"/>
+      <c r="B872" s="5"/>
     </row>
     <row r="873" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A873" s="5"/>
-      <c r="B873" s="6"/>
+      <c r="A873" s="4"/>
+      <c r="B873" s="5"/>
     </row>
     <row r="874" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A874" s="5"/>
-      <c r="B874" s="6"/>
+      <c r="A874" s="4"/>
+      <c r="B874" s="5"/>
     </row>
     <row r="875" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A875" s="5"/>
-      <c r="B875" s="6"/>
+      <c r="A875" s="4"/>
+      <c r="B875" s="5"/>
     </row>
     <row r="876" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A876" s="5"/>
-      <c r="B876" s="6"/>
+      <c r="A876" s="4"/>
+      <c r="B876" s="5"/>
     </row>
     <row r="877" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A877" s="5"/>
-      <c r="B877" s="6"/>
+      <c r="A877" s="4"/>
+      <c r="B877" s="5"/>
     </row>
     <row r="878" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A878" s="5"/>
-      <c r="B878" s="6"/>
+      <c r="A878" s="4"/>
+      <c r="B878" s="5"/>
     </row>
     <row r="879" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A879" s="5"/>
-      <c r="B879" s="6"/>
+      <c r="A879" s="4"/>
+      <c r="B879" s="5"/>
     </row>
     <row r="880" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A880" s="5"/>
-      <c r="B880" s="6"/>
+      <c r="A880" s="4"/>
+      <c r="B880" s="5"/>
     </row>
     <row r="881" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A881" s="5"/>
-      <c r="B881" s="6"/>
+      <c r="A881" s="4"/>
+      <c r="B881" s="5"/>
     </row>
     <row r="882" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A882" s="5"/>
-      <c r="B882" s="6"/>
+      <c r="A882" s="4"/>
+      <c r="B882" s="5"/>
     </row>
     <row r="883" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A883" s="5"/>
-      <c r="B883" s="6"/>
+      <c r="A883" s="4"/>
+      <c r="B883" s="5"/>
     </row>
     <row r="884" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A884" s="5"/>
-      <c r="B884" s="6"/>
+      <c r="A884" s="4"/>
+      <c r="B884" s="5"/>
     </row>
     <row r="885" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A885" s="5"/>
-      <c r="B885" s="6"/>
+      <c r="A885" s="4"/>
+      <c r="B885" s="5"/>
     </row>
     <row r="886" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A886" s="5"/>
-      <c r="B886" s="6"/>
+      <c r="A886" s="4"/>
+      <c r="B886" s="5"/>
     </row>
     <row r="887" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A887" s="5"/>
-      <c r="B887" s="6"/>
+      <c r="A887" s="4"/>
+      <c r="B887" s="5"/>
     </row>
     <row r="888" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A888" s="5"/>
-      <c r="B888" s="6"/>
+      <c r="A888" s="4"/>
+      <c r="B888" s="5"/>
     </row>
     <row r="889" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A889" s="5"/>
-      <c r="B889" s="6"/>
+      <c r="A889" s="4"/>
+      <c r="B889" s="5"/>
     </row>
     <row r="890" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A890" s="5"/>
-      <c r="B890" s="6"/>
+      <c r="A890" s="4"/>
+      <c r="B890" s="5"/>
     </row>
     <row r="891" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A891" s="5"/>
-      <c r="B891" s="6"/>
+      <c r="A891" s="4"/>
+      <c r="B891" s="5"/>
     </row>
     <row r="892" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A892" s="5"/>
-      <c r="B892" s="6"/>
+      <c r="A892" s="4"/>
+      <c r="B892" s="5"/>
     </row>
     <row r="893" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A893" s="5"/>
-      <c r="B893" s="6"/>
+      <c r="A893" s="4"/>
+      <c r="B893" s="5"/>
     </row>
     <row r="894" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A894" s="5"/>
-      <c r="B894" s="6"/>
+      <c r="A894" s="4"/>
+      <c r="B894" s="5"/>
     </row>
     <row r="895" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A895" s="5"/>
-      <c r="B895" s="6"/>
+      <c r="A895" s="4"/>
+      <c r="B895" s="5"/>
     </row>
     <row r="896" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A896" s="5"/>
-      <c r="B896" s="6"/>
+      <c r="A896" s="4"/>
+      <c r="B896" s="5"/>
     </row>
     <row r="897" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A897" s="5"/>
-      <c r="B897" s="6"/>
+      <c r="A897" s="4"/>
+      <c r="B897" s="5"/>
     </row>
     <row r="898" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A898" s="5"/>
-      <c r="B898" s="6"/>
+      <c r="A898" s="4"/>
+      <c r="B898" s="5"/>
     </row>
     <row r="899" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A899" s="5"/>
-      <c r="B899" s="6"/>
+      <c r="A899" s="4"/>
+      <c r="B899" s="5"/>
     </row>
     <row r="900" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A900" s="5"/>
-      <c r="B900" s="6"/>
+      <c r="A900" s="4"/>
+      <c r="B900" s="5"/>
     </row>
     <row r="901" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A901" s="5"/>
-      <c r="B901" s="6"/>
+      <c r="A901" s="4"/>
+      <c r="B901" s="5"/>
     </row>
     <row r="902" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A902" s="5"/>
-      <c r="B902" s="6"/>
+      <c r="A902" s="4"/>
+      <c r="B902" s="5"/>
     </row>
     <row r="903" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A903" s="5"/>
-      <c r="B903" s="6"/>
+      <c r="A903" s="4"/>
+      <c r="B903" s="5"/>
     </row>
     <row r="904" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A904" s="5"/>
-      <c r="B904" s="6"/>
+      <c r="A904" s="4"/>
+      <c r="B904" s="5"/>
     </row>
     <row r="905" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A905" s="5"/>
-      <c r="B905" s="6"/>
+      <c r="A905" s="4"/>
+      <c r="B905" s="5"/>
     </row>
     <row r="906" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A906" s="5"/>
-      <c r="B906" s="6"/>
+      <c r="A906" s="4"/>
+      <c r="B906" s="5"/>
     </row>
     <row r="907" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A907" s="5"/>
-      <c r="B907" s="6"/>
+      <c r="A907" s="4"/>
+      <c r="B907" s="5"/>
     </row>
     <row r="908" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A908" s="5"/>
-      <c r="B908" s="6"/>
+      <c r="A908" s="4"/>
+      <c r="B908" s="5"/>
     </row>
     <row r="909" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A909" s="5"/>
-      <c r="B909" s="6"/>
+      <c r="A909" s="4"/>
+      <c r="B909" s="5"/>
     </row>
     <row r="910" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A910" s="5"/>
-      <c r="B910" s="6"/>
+      <c r="A910" s="4"/>
+      <c r="B910" s="5"/>
     </row>
     <row r="911" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A911" s="5"/>
-      <c r="B911" s="6"/>
+      <c r="A911" s="4"/>
+      <c r="B911" s="5"/>
     </row>
     <row r="912" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A912" s="5"/>
-      <c r="B912" s="6"/>
+      <c r="A912" s="4"/>
+      <c r="B912" s="5"/>
     </row>
     <row r="913" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A913" s="5"/>
-      <c r="B913" s="6"/>
+      <c r="A913" s="4"/>
+      <c r="B913" s="5"/>
     </row>
     <row r="914" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A914" s="5"/>
-      <c r="B914" s="6"/>
+      <c r="A914" s="4"/>
+      <c r="B914" s="5"/>
     </row>
     <row r="915" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A915" s="5"/>
-      <c r="B915" s="6"/>
+      <c r="A915" s="4"/>
+      <c r="B915" s="5"/>
     </row>
     <row r="916" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A916" s="5"/>
-      <c r="B916" s="6"/>
+      <c r="A916" s="4"/>
+      <c r="B916" s="5"/>
     </row>
     <row r="917" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A917" s="5"/>
-      <c r="B917" s="6"/>
+      <c r="A917" s="4"/>
+      <c r="B917" s="5"/>
     </row>
     <row r="918" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A918" s="5"/>
-      <c r="B918" s="6"/>
+      <c r="A918" s="4"/>
+      <c r="B918" s="5"/>
     </row>
     <row r="919" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A919" s="5"/>
-      <c r="B919" s="6"/>
+      <c r="A919" s="4"/>
+      <c r="B919" s="5"/>
     </row>
     <row r="920" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A920" s="5"/>
-      <c r="B920" s="6"/>
+      <c r="A920" s="4"/>
+      <c r="B920" s="5"/>
     </row>
     <row r="921" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A921" s="5"/>
-      <c r="B921" s="6"/>
+      <c r="A921" s="4"/>
+      <c r="B921" s="5"/>
     </row>
     <row r="922" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A922" s="5"/>
-      <c r="B922" s="6"/>
+      <c r="A922" s="4"/>
+      <c r="B922" s="5"/>
     </row>
     <row r="923" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A923" s="5"/>
-      <c r="B923" s="6"/>
+      <c r="A923" s="4"/>
+      <c r="B923" s="5"/>
     </row>
     <row r="924" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A924" s="5"/>
-      <c r="B924" s="6"/>
+      <c r="A924" s="4"/>
+      <c r="B924" s="5"/>
     </row>
     <row r="925" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A925" s="5"/>
-      <c r="B925" s="6"/>
+      <c r="A925" s="4"/>
+      <c r="B925" s="5"/>
     </row>
     <row r="926" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A926" s="5"/>
-      <c r="B926" s="6"/>
+      <c r="A926" s="4"/>
+      <c r="B926" s="5"/>
     </row>
     <row r="927" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A927" s="5"/>
-      <c r="B927" s="6"/>
+      <c r="A927" s="4"/>
+      <c r="B927" s="5"/>
     </row>
     <row r="928" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A928" s="5"/>
-      <c r="B928" s="6"/>
+      <c r="A928" s="4"/>
+      <c r="B928" s="5"/>
     </row>
     <row r="929" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A929" s="5"/>
-      <c r="B929" s="6"/>
+      <c r="A929" s="4"/>
+      <c r="B929" s="5"/>
     </row>
     <row r="930" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A930" s="5"/>
-      <c r="B930" s="6"/>
+      <c r="A930" s="4"/>
+      <c r="B930" s="5"/>
     </row>
     <row r="931" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A931" s="5"/>
-      <c r="B931" s="6"/>
+      <c r="A931" s="4"/>
+      <c r="B931" s="5"/>
     </row>
     <row r="932" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A932" s="5"/>
-      <c r="B932" s="6"/>
+      <c r="A932" s="4"/>
+      <c r="B932" s="5"/>
     </row>
     <row r="933" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A933" s="5"/>
-      <c r="B933" s="6"/>
+      <c r="A933" s="4"/>
+      <c r="B933" s="5"/>
     </row>
     <row r="934" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A934" s="5"/>
-      <c r="B934" s="6"/>
+      <c r="A934" s="4"/>
+      <c r="B934" s="5"/>
     </row>
     <row r="935" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A935" s="5"/>
-      <c r="B935" s="6"/>
+      <c r="A935" s="4"/>
+      <c r="B935" s="5"/>
     </row>
     <row r="936" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A936" s="5"/>
-      <c r="B936" s="6"/>
+      <c r="A936" s="4"/>
+      <c r="B936" s="5"/>
     </row>
     <row r="937" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A937" s="5"/>
-      <c r="B937" s="6"/>
+      <c r="A937" s="4"/>
+      <c r="B937" s="5"/>
     </row>
     <row r="938" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A938" s="5"/>
-      <c r="B938" s="6"/>
+      <c r="A938" s="4"/>
+      <c r="B938" s="5"/>
     </row>
     <row r="939" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A939" s="5"/>
-      <c r="B939" s="6"/>
+      <c r="A939" s="4"/>
+      <c r="B939" s="5"/>
     </row>
     <row r="940" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A940" s="5"/>
-      <c r="B940" s="6"/>
+      <c r="A940" s="4"/>
+      <c r="B940" s="5"/>
     </row>
     <row r="941" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A941" s="5"/>
-      <c r="B941" s="6"/>
+      <c r="A941" s="4"/>
+      <c r="B941" s="5"/>
     </row>
     <row r="942" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A942" s="5"/>
-      <c r="B942" s="6"/>
+      <c r="A942" s="4"/>
+      <c r="B942" s="5"/>
     </row>
     <row r="943" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A943" s="5"/>
-      <c r="B943" s="6"/>
+      <c r="A943" s="4"/>
+      <c r="B943" s="5"/>
     </row>
     <row r="944" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A944" s="5"/>
-      <c r="B944" s="6"/>
+      <c r="A944" s="4"/>
+      <c r="B944" s="5"/>
     </row>
     <row r="945" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A945" s="5"/>
-      <c r="B945" s="6"/>
+      <c r="A945" s="4"/>
+      <c r="B945" s="5"/>
     </row>
     <row r="946" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A946" s="5"/>
-      <c r="B946" s="6"/>
+      <c r="A946" s="4"/>
+      <c r="B946" s="5"/>
     </row>
     <row r="947" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A947" s="5"/>
-      <c r="B947" s="6"/>
+      <c r="A947" s="4"/>
+      <c r="B947" s="5"/>
     </row>
     <row r="948" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A948" s="5"/>
-      <c r="B948" s="6"/>
+      <c r="A948" s="4"/>
+      <c r="B948" s="5"/>
     </row>
     <row r="949" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A949" s="5"/>
-      <c r="B949" s="6"/>
+      <c r="A949" s="4"/>
+      <c r="B949" s="5"/>
     </row>
     <row r="950" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A950" s="5"/>
-      <c r="B950" s="6"/>
+      <c r="A950" s="4"/>
+      <c r="B950" s="5"/>
     </row>
     <row r="951" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A951" s="5"/>
-      <c r="B951" s="6"/>
+      <c r="A951" s="4"/>
+      <c r="B951" s="5"/>
     </row>
     <row r="952" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A952" s="5"/>
-      <c r="B952" s="6"/>
+      <c r="A952" s="4"/>
+      <c r="B952" s="5"/>
     </row>
     <row r="953" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A953" s="5"/>
-      <c r="B953" s="6"/>
+      <c r="A953" s="4"/>
+      <c r="B953" s="5"/>
     </row>
     <row r="954" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A954" s="5"/>
-      <c r="B954" s="6"/>
+      <c r="A954" s="4"/>
+      <c r="B954" s="5"/>
     </row>
     <row r="955" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A955" s="5"/>
-      <c r="B955" s="6"/>
+      <c r="A955" s="4"/>
+      <c r="B955" s="5"/>
     </row>
     <row r="956" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A956" s="5"/>
-      <c r="B956" s="6"/>
+      <c r="A956" s="4"/>
+      <c r="B956" s="5"/>
     </row>
     <row r="957" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A957" s="5"/>
-      <c r="B957" s="6"/>
+      <c r="A957" s="4"/>
+      <c r="B957" s="5"/>
     </row>
     <row r="958" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A958" s="5"/>
-      <c r="B958" s="6"/>
+      <c r="A958" s="4"/>
+      <c r="B958" s="5"/>
     </row>
     <row r="959" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A959" s="5"/>
-      <c r="B959" s="6"/>
+      <c r="A959" s="4"/>
+      <c r="B959" s="5"/>
     </row>
     <row r="960" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A960" s="5"/>
-      <c r="B960" s="6"/>
+      <c r="A960" s="4"/>
+      <c r="B960" s="5"/>
     </row>
     <row r="961" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A961" s="5"/>
-      <c r="B961" s="6"/>
+      <c r="A961" s="4"/>
+      <c r="B961" s="5"/>
     </row>
     <row r="962" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A962" s="5"/>
-      <c r="B962" s="6"/>
+      <c r="A962" s="4"/>
+      <c r="B962" s="5"/>
     </row>
     <row r="963" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A963" s="5"/>
-      <c r="B963" s="6"/>
+      <c r="A963" s="4"/>
+      <c r="B963" s="5"/>
     </row>
     <row r="964" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A964" s="5"/>
-      <c r="B964" s="6"/>
+      <c r="A964" s="4"/>
+      <c r="B964" s="5"/>
     </row>
     <row r="965" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A965" s="5"/>
-      <c r="B965" s="6"/>
+      <c r="A965" s="4"/>
+      <c r="B965" s="5"/>
     </row>
     <row r="966" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A966" s="5"/>
-      <c r="B966" s="6"/>
+      <c r="A966" s="4"/>
+      <c r="B966" s="5"/>
     </row>
     <row r="967" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A967" s="5"/>
-      <c r="B967" s="6"/>
+      <c r="A967" s="4"/>
+      <c r="B967" s="5"/>
     </row>
     <row r="968" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A968" s="5"/>
-      <c r="B968" s="6"/>
+      <c r="A968" s="4"/>
+      <c r="B968" s="5"/>
     </row>
     <row r="969" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A969" s="5"/>
-      <c r="B969" s="6"/>
+      <c r="A969" s="4"/>
+      <c r="B969" s="5"/>
     </row>
     <row r="970" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A970" s="5"/>
-      <c r="B970" s="6"/>
+      <c r="A970" s="4"/>
+      <c r="B970" s="5"/>
     </row>
     <row r="971" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A971" s="5"/>
-      <c r="B971" s="6"/>
+      <c r="A971" s="4"/>
+      <c r="B971" s="5"/>
     </row>
     <row r="972" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A972" s="5"/>
-      <c r="B972" s="6"/>
+      <c r="A972" s="4"/>
+      <c r="B972" s="5"/>
     </row>
     <row r="973" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A973" s="5"/>
-      <c r="B973" s="6"/>
+      <c r="A973" s="4"/>
+      <c r="B973" s="5"/>
     </row>
     <row r="974" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A974" s="5"/>
-      <c r="B974" s="6"/>
+      <c r="A974" s="4"/>
+      <c r="B974" s="5"/>
     </row>
     <row r="975" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A975" s="5"/>
-      <c r="B975" s="6"/>
+      <c r="A975" s="4"/>
+      <c r="B975" s="5"/>
     </row>
     <row r="976" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A976" s="5"/>
-      <c r="B976" s="6"/>
+      <c r="A976" s="4"/>
+      <c r="B976" s="5"/>
     </row>
     <row r="977" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A977" s="5"/>
-      <c r="B977" s="6"/>
+      <c r="A977" s="4"/>
+      <c r="B977" s="5"/>
     </row>
     <row r="978" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A978" s="5"/>
-      <c r="B978" s="6"/>
+      <c r="A978" s="4"/>
+      <c r="B978" s="5"/>
     </row>
     <row r="979" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A979" s="5"/>
-      <c r="B979" s="6"/>
+      <c r="A979" s="4"/>
+      <c r="B979" s="5"/>
     </row>
     <row r="980" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A980" s="5"/>
-      <c r="B980" s="6"/>
+      <c r="A980" s="4"/>
+      <c r="B980" s="5"/>
     </row>
     <row r="981" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A981" s="5"/>
-      <c r="B981" s="6"/>
+      <c r="A981" s="4"/>
+      <c r="B981" s="5"/>
     </row>
     <row r="982" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A982" s="5"/>
-      <c r="B982" s="6"/>
+      <c r="A982" s="4"/>
+      <c r="B982" s="5"/>
     </row>
     <row r="983" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A983" s="5"/>
-      <c r="B983" s="6"/>
+      <c r="A983" s="4"/>
+      <c r="B983" s="5"/>
     </row>
     <row r="984" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A984" s="5"/>
-      <c r="B984" s="6"/>
+      <c r="A984" s="4"/>
+      <c r="B984" s="5"/>
     </row>
     <row r="985" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A985" s="5"/>
-      <c r="B985" s="6"/>
+      <c r="A985" s="4"/>
+      <c r="B985" s="5"/>
     </row>
     <row r="986" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A986" s="5"/>
-      <c r="B986" s="6"/>
+      <c r="A986" s="4"/>
+      <c r="B986" s="5"/>
     </row>
     <row r="987" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A987" s="5"/>
-      <c r="B987" s="6"/>
+      <c r="A987" s="4"/>
+      <c r="B987" s="5"/>
     </row>
     <row r="988" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A988" s="5"/>
-      <c r="B988" s="6"/>
+      <c r="A988" s="4"/>
+      <c r="B988" s="5"/>
     </row>
     <row r="989" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A989" s="5"/>
-      <c r="B989" s="6"/>
+      <c r="A989" s="4"/>
+      <c r="B989" s="5"/>
     </row>
     <row r="990" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A990" s="5"/>
-      <c r="B990" s="6"/>
+      <c r="A990" s="4"/>
+      <c r="B990" s="5"/>
     </row>
     <row r="991" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A991" s="5"/>
-      <c r="B991" s="6"/>
+      <c r="A991" s="4"/>
+      <c r="B991" s="5"/>
     </row>
     <row r="992" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A992" s="5"/>
-      <c r="B992" s="6"/>
+      <c r="A992" s="4"/>
+      <c r="B992" s="5"/>
     </row>
     <row r="993" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A993" s="5"/>
-      <c r="B993" s="6"/>
+      <c r="A993" s="4"/>
+      <c r="B993" s="5"/>
     </row>
     <row r="994" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A994" s="5"/>
-      <c r="B994" s="6"/>
+      <c r="A994" s="4"/>
+      <c r="B994" s="5"/>
     </row>
     <row r="995" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A995" s="5"/>
-      <c r="B995" s="6"/>
+      <c r="A995" s="4"/>
+      <c r="B995" s="5"/>
     </row>
     <row r="996" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A996" s="5"/>
-      <c r="B996" s="6"/>
+      <c r="A996" s="4"/>
+      <c r="B996" s="5"/>
     </row>
     <row r="997" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A997" s="5"/>
-      <c r="B997" s="6"/>
+      <c r="A997" s="4"/>
+      <c r="B997" s="5"/>
     </row>
     <row r="998" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A998" s="5"/>
-      <c r="B998" s="6"/>
+      <c r="A998" s="4"/>
+      <c r="B998" s="5"/>
     </row>
     <row r="999" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A999" s="5"/>
-      <c r="B999" s="6"/>
+      <c r="A999" s="4"/>
+      <c r="B999" s="5"/>
     </row>
     <row r="1000" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1000" s="5"/>
-      <c r="B1000" s="6"/>
+      <c r="A1000" s="4"/>
+      <c r="B1000" s="5"/>
     </row>
     <row r="1001" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1001" s="5"/>
-      <c r="B1001" s="6"/>
+      <c r="A1001" s="4"/>
+      <c r="B1001" s="5"/>
     </row>
     <row r="1002" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1002" s="5"/>
-      <c r="B1002" s="6"/>
+      <c r="A1002" s="4"/>
+      <c r="B1002" s="5"/>
     </row>
     <row r="1003" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1003" s="5"/>
-      <c r="B1003" s="6"/>
+      <c r="A1003" s="4"/>
+      <c r="B1003" s="5"/>
     </row>
     <row r="1004" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1004" s="5"/>
-      <c r="B1004" s="6"/>
+      <c r="A1004" s="4"/>
+      <c r="B1004" s="5"/>
     </row>
     <row r="1005" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1005" s="5"/>
-      <c r="B1005" s="6"/>
+      <c r="A1005" s="4"/>
+      <c r="B1005" s="5"/>
     </row>
     <row r="1006" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1006" s="5"/>
-      <c r="B1006" s="6"/>
+      <c r="A1006" s="4"/>
+      <c r="B1006" s="5"/>
     </row>
     <row r="1007" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1007" s="5"/>
-      <c r="B1007" s="6"/>
+      <c r="A1007" s="4"/>
+      <c r="B1007" s="5"/>
     </row>
     <row r="1008" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1008" s="5"/>
-      <c r="B1008" s="6"/>
+      <c r="A1008" s="4"/>
+      <c r="B1008" s="5"/>
     </row>
     <row r="1009" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1009" s="5"/>
-      <c r="B1009" s="6"/>
+      <c r="A1009" s="4"/>
+      <c r="B1009" s="5"/>
     </row>
     <row r="1010" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1010" s="5"/>
-      <c r="B1010" s="6"/>
+      <c r="A1010" s="4"/>
+      <c r="B1010" s="5"/>
     </row>
     <row r="1011" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1011" s="5"/>
-      <c r="B1011" s="6"/>
+      <c r="A1011" s="4"/>
+      <c r="B1011" s="5"/>
     </row>
     <row r="1012" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1012" s="5"/>
-      <c r="B1012" s="6"/>
+      <c r="A1012" s="4"/>
+      <c r="B1012" s="5"/>
     </row>
     <row r="1013" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1013" s="5"/>
-      <c r="B1013" s="6"/>
+      <c r="A1013" s="4"/>
+      <c r="B1013" s="5"/>
     </row>
     <row r="1014" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1014" s="5"/>
-      <c r="B1014" s="6"/>
+      <c r="A1014" s="4"/>
+      <c r="B1014" s="5"/>
     </row>
     <row r="1015" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1015" s="5"/>
-      <c r="B1015" s="6"/>
+      <c r="A1015" s="4"/>
+      <c r="B1015" s="5"/>
     </row>
     <row r="1016" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1016" s="5"/>
-      <c r="B1016" s="6"/>
+      <c r="A1016" s="4"/>
+      <c r="B1016" s="5"/>
     </row>
     <row r="1017" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1017" s="5"/>
-      <c r="B1017" s="6"/>
+      <c r="A1017" s="4"/>
+      <c r="B1017" s="5"/>
     </row>
     <row r="1018" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1018" s="5"/>
-      <c r="B1018" s="6"/>
+      <c r="A1018" s="4"/>
+      <c r="B1018" s="5"/>
     </row>
     <row r="1019" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1019" s="5"/>
-      <c r="B1019" s="6"/>
+      <c r="A1019" s="4"/>
+      <c r="B1019" s="5"/>
     </row>
     <row r="1020" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1020" s="5"/>
-      <c r="B1020" s="6"/>
+      <c r="A1020" s="4"/>
+      <c r="B1020" s="5"/>
     </row>
     <row r="1021" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1021" s="5"/>
-      <c r="B1021" s="6"/>
+      <c r="A1021" s="4"/>
+      <c r="B1021" s="5"/>
     </row>
     <row r="1022" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1022" s="5"/>
-      <c r="B1022" s="6"/>
+      <c r="A1022" s="4"/>
+      <c r="B1022" s="5"/>
     </row>
     <row r="1023" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1023" s="5"/>
-      <c r="B1023" s="6"/>
+      <c r="A1023" s="4"/>
+      <c r="B1023" s="5"/>
     </row>
     <row r="1024" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1024" s="5"/>
-      <c r="B1024" s="6"/>
+      <c r="A1024" s="4"/>
+      <c r="B1024" s="5"/>
     </row>
     <row r="1025" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1025" s="5"/>
-      <c r="B1025" s="6"/>
+      <c r="A1025" s="4"/>
+      <c r="B1025" s="5"/>
     </row>
     <row r="1026" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1026" s="5"/>
-      <c r="B1026" s="6"/>
+      <c r="A1026" s="4"/>
+      <c r="B1026" s="5"/>
     </row>
     <row r="1027" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1027" s="5"/>
-      <c r="B1027" s="6"/>
+      <c r="A1027" s="4"/>
+      <c r="B1027" s="5"/>
     </row>
     <row r="1028" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1028" s="5"/>
-      <c r="B1028" s="6"/>
+      <c r="A1028" s="4"/>
+      <c r="B1028" s="5"/>
     </row>
     <row r="1029" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1029" s="5"/>
-      <c r="B1029" s="6"/>
+      <c r="A1029" s="4"/>
+      <c r="B1029" s="5"/>
     </row>
     <row r="1030" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1030" s="5"/>
-      <c r="B1030" s="6"/>
+      <c r="A1030" s="4"/>
+      <c r="B1030" s="5"/>
     </row>
     <row r="1031" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1031" s="5"/>
-      <c r="B1031" s="6"/>
+      <c r="A1031" s="4"/>
+      <c r="B1031" s="5"/>
     </row>
     <row r="1032" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1032" s="5"/>
-      <c r="B1032" s="6"/>
+      <c r="A1032" s="4"/>
+      <c r="B1032" s="5"/>
     </row>
     <row r="1033" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1033" s="5"/>
-      <c r="B1033" s="6"/>
+      <c r="A1033" s="4"/>
+      <c r="B1033" s="5"/>
     </row>
     <row r="1034" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1034" s="5"/>
-      <c r="B1034" s="6"/>
+      <c r="A1034" s="4"/>
+      <c r="B1034" s="5"/>
     </row>
     <row r="1035" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1035" s="5"/>
-      <c r="B1035" s="6"/>
+      <c r="A1035" s="4"/>
+      <c r="B1035" s="5"/>
     </row>
     <row r="1036" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1036" s="5"/>
-      <c r="B1036" s="6"/>
+      <c r="A1036" s="4"/>
+      <c r="B1036" s="5"/>
     </row>
     <row r="1037" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1037" s="5"/>
-      <c r="B1037" s="6"/>
+      <c r="A1037" s="4"/>
+      <c r="B1037" s="5"/>
     </row>
     <row r="1038" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1038" s="5"/>
-      <c r="B1038" s="6"/>
+      <c r="A1038" s="4"/>
+      <c r="B1038" s="5"/>
     </row>
     <row r="1039" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1039" s="5"/>
-      <c r="B1039" s="6"/>
+      <c r="A1039" s="4"/>
+      <c r="B1039" s="5"/>
     </row>
     <row r="1040" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1040" s="5"/>
-      <c r="B1040" s="6"/>
+      <c r="A1040" s="4"/>
+      <c r="B1040" s="5"/>
     </row>
     <row r="1041" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1041" s="5"/>
-      <c r="B1041" s="6"/>
+      <c r="A1041" s="4"/>
+      <c r="B1041" s="5"/>
     </row>
     <row r="1042" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1042" s="5"/>
-      <c r="B1042" s="6"/>
+      <c r="A1042" s="4"/>
+      <c r="B1042" s="5"/>
     </row>
     <row r="1043" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1043" s="5"/>
-      <c r="B1043" s="6"/>
+      <c r="A1043" s="4"/>
+      <c r="B1043" s="5"/>
     </row>
     <row r="1044" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1044" s="5"/>
-      <c r="B1044" s="6"/>
+      <c r="A1044" s="4"/>
+      <c r="B1044" s="5"/>
     </row>
     <row r="1045" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1045" s="5"/>
-      <c r="B1045" s="6"/>
+      <c r="A1045" s="4"/>
+      <c r="B1045" s="5"/>
     </row>
     <row r="1046" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1046" s="5"/>
-      <c r="B1046" s="6"/>
+      <c r="A1046" s="4"/>
+      <c r="B1046" s="5"/>
     </row>
     <row r="1047" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1047" s="5"/>
-      <c r="B1047" s="6"/>
+      <c r="A1047" s="4"/>
+      <c r="B1047" s="5"/>
     </row>
     <row r="1048" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1048" s="5"/>
-      <c r="B1048" s="6"/>
+      <c r="A1048" s="4"/>
+      <c r="B1048" s="5"/>
     </row>
     <row r="1049" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1049" s="5"/>
-      <c r="B1049" s="6"/>
+      <c r="A1049" s="4"/>
+      <c r="B1049" s="5"/>
     </row>
     <row r="1050" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1050" s="5"/>
-      <c r="B1050" s="6"/>
+      <c r="A1050" s="4"/>
+      <c r="B1050" s="5"/>
     </row>
     <row r="1051" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1051" s="5"/>
-      <c r="B1051" s="6"/>
+      <c r="A1051" s="4"/>
+      <c r="B1051" s="5"/>
     </row>
     <row r="1052" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1052" s="5"/>
-      <c r="B1052" s="6"/>
+      <c r="A1052" s="4"/>
+      <c r="B1052" s="5"/>
     </row>
     <row r="1053" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1053" s="5"/>
-      <c r="B1053" s="6"/>
+      <c r="A1053" s="4"/>
+      <c r="B1053" s="5"/>
     </row>
     <row r="1054" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1054" s="5"/>
-      <c r="B1054" s="6"/>
+      <c r="A1054" s="4"/>
+      <c r="B1054" s="5"/>
     </row>
     <row r="1055" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1055" s="5"/>
-      <c r="B1055" s="6"/>
+      <c r="A1055" s="4"/>
+      <c r="B1055" s="5"/>
     </row>
     <row r="1056" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1056" s="5"/>
-      <c r="B1056" s="6"/>
+      <c r="A1056" s="4"/>
+      <c r="B1056" s="5"/>
     </row>
     <row r="1057" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1057" s="5"/>
-      <c r="B1057" s="6"/>
+      <c r="A1057" s="4"/>
+      <c r="B1057" s="5"/>
     </row>
     <row r="1058" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1058" s="5"/>
-      <c r="B1058" s="6"/>
+      <c r="A1058" s="4"/>
+      <c r="B1058" s="5"/>
     </row>
     <row r="1059" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1059" s="5"/>
-      <c r="B1059" s="6"/>
+      <c r="A1059" s="4"/>
+      <c r="B1059" s="5"/>
     </row>
     <row r="1060" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1060" s="5"/>
-      <c r="B1060" s="6"/>
+      <c r="A1060" s="4"/>
+      <c r="B1060" s="5"/>
     </row>
     <row r="1061" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1061" s="5"/>
-      <c r="B1061" s="6"/>
+      <c r="A1061" s="4"/>
+      <c r="B1061" s="5"/>
     </row>
     <row r="1062" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1062" s="5"/>
-      <c r="B1062" s="6"/>
+      <c r="A1062" s="4"/>
+      <c r="B1062" s="5"/>
     </row>
     <row r="1063" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1063" s="5"/>
-      <c r="B1063" s="6"/>
+      <c r="A1063" s="4"/>
+      <c r="B1063" s="5"/>
     </row>
     <row r="1064" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1064" s="5"/>
-      <c r="B1064" s="6"/>
+      <c r="A1064" s="4"/>
+      <c r="B1064" s="5"/>
     </row>
     <row r="1065" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1065" s="5"/>
-      <c r="B1065" s="6"/>
+      <c r="A1065" s="4"/>
+      <c r="B1065" s="5"/>
     </row>
     <row r="1066" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1066" s="5"/>
-      <c r="B1066" s="6"/>
+      <c r="A1066" s="4"/>
+      <c r="B1066" s="5"/>
     </row>
     <row r="1067" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1067" s="5"/>
-      <c r="B1067" s="6"/>
+      <c r="A1067" s="4"/>
+      <c r="B1067" s="5"/>
     </row>
     <row r="1068" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1068" s="5"/>
-      <c r="B1068" s="6"/>
+      <c r="A1068" s="4"/>
+      <c r="B1068" s="5"/>
     </row>
     <row r="1069" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1069" s="5"/>
-      <c r="B1069" s="6"/>
+      <c r="A1069" s="4"/>
+      <c r="B1069" s="5"/>
     </row>
     <row r="1070" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1070" s="5"/>
-      <c r="B1070" s="6"/>
+      <c r="A1070" s="4"/>
+      <c r="B1070" s="5"/>
     </row>
     <row r="1071" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1071" s="5"/>
-      <c r="B1071" s="6"/>
+      <c r="A1071" s="4"/>
+      <c r="B1071" s="5"/>
     </row>
     <row r="1072" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1072" s="5"/>
-      <c r="B1072" s="6"/>
+      <c r="A1072" s="4"/>
+      <c r="B1072" s="5"/>
     </row>
     <row r="1073" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1073" s="5"/>
-      <c r="B1073" s="6"/>
+      <c r="A1073" s="4"/>
+      <c r="B1073" s="5"/>
     </row>
     <row r="1074" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1074" s="5"/>
-      <c r="B1074" s="6"/>
+      <c r="A1074" s="4"/>
+      <c r="B1074" s="5"/>
     </row>
     <row r="1075" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1075" s="5"/>
-      <c r="B1075" s="6"/>
+      <c r="A1075" s="4"/>
+      <c r="B1075" s="5"/>
     </row>
     <row r="1076" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1076" s="5"/>
-      <c r="B1076" s="6"/>
+      <c r="A1076" s="4"/>
+      <c r="B1076" s="5"/>
     </row>
     <row r="1077" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1077" s="5"/>
-      <c r="B1077" s="6"/>
+      <c r="A1077" s="4"/>
+      <c r="B1077" s="5"/>
     </row>
     <row r="1078" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1078" s="5"/>
-      <c r="B1078" s="6"/>
+      <c r="A1078" s="4"/>
+      <c r="B1078" s="5"/>
     </row>
     <row r="1079" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1079" s="5"/>
-      <c r="B1079" s="6"/>
+      <c r="A1079" s="4"/>
+      <c r="B1079" s="5"/>
     </row>
     <row r="1080" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1080" s="5"/>
-      <c r="B1080" s="6"/>
+      <c r="A1080" s="4"/>
+      <c r="B1080" s="5"/>
     </row>
     <row r="1081" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1081" s="5"/>
-      <c r="B1081" s="6"/>
+      <c r="A1081" s="4"/>
+      <c r="B1081" s="5"/>
     </row>
     <row r="1082" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1082" s="5"/>
-      <c r="B1082" s="6"/>
+      <c r="A1082" s="4"/>
+      <c r="B1082" s="5"/>
     </row>
     <row r="1083" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1083" s="5"/>
-      <c r="B1083" s="6"/>
+      <c r="A1083" s="4"/>
+      <c r="B1083" s="5"/>
     </row>
     <row r="1084" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1084" s="5"/>
-      <c r="B1084" s="6"/>
+      <c r="A1084" s="4"/>
+      <c r="B1084" s="5"/>
     </row>
     <row r="1085" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1085" s="5"/>
-      <c r="B1085" s="6"/>
+      <c r="A1085" s="4"/>
+      <c r="B1085" s="5"/>
     </row>
     <row r="1086" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1086" s="5"/>
-      <c r="B1086" s="6"/>
+      <c r="A1086" s="4"/>
+      <c r="B1086" s="5"/>
     </row>
     <row r="1087" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1087" s="5"/>
-      <c r="B1087" s="6"/>
+      <c r="A1087" s="4"/>
+      <c r="B1087" s="5"/>
     </row>
     <row r="1088" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1088" s="5"/>
-      <c r="B1088" s="6"/>
+      <c r="A1088" s="4"/>
+      <c r="B1088" s="5"/>
     </row>
     <row r="1089" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1089" s="5"/>
-      <c r="B1089" s="6"/>
+      <c r="A1089" s="4"/>
+      <c r="B1089" s="5"/>
     </row>
     <row r="1090" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1090" s="5"/>
-      <c r="B1090" s="6"/>
+      <c r="A1090" s="4"/>
+      <c r="B1090" s="5"/>
     </row>
     <row r="1091" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1091" s="5"/>
-      <c r="B1091" s="6"/>
+      <c r="A1091" s="4"/>
+      <c r="B1091" s="5"/>
     </row>
     <row r="1092" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1092" s="5"/>
-      <c r="B1092" s="6"/>
+      <c r="A1092" s="4"/>
+      <c r="B1092" s="5"/>
     </row>
     <row r="1093" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1093" s="5"/>
-      <c r="B1093" s="6"/>
+      <c r="A1093" s="4"/>
+      <c r="B1093" s="5"/>
     </row>
     <row r="1094" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1094" s="5"/>
-      <c r="B1094" s="6"/>
+      <c r="A1094" s="4"/>
+      <c r="B1094" s="5"/>
     </row>
     <row r="1095" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1095" s="5"/>
-      <c r="B1095" s="6"/>
+      <c r="A1095" s="4"/>
+      <c r="B1095" s="5"/>
     </row>
     <row r="1096" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1096" s="5"/>
-      <c r="B1096" s="6"/>
+      <c r="A1096" s="4"/>
+      <c r="B1096" s="5"/>
     </row>
     <row r="1097" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1097" s="5"/>
-      <c r="B1097" s="6"/>
+      <c r="A1097" s="4"/>
+      <c r="B1097" s="5"/>
     </row>
     <row r="1098" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1098" s="5"/>
-      <c r="B1098" s="6"/>
+      <c r="A1098" s="4"/>
+      <c r="B1098" s="5"/>
     </row>
     <row r="1099" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1099" s="5"/>
-      <c r="B1099" s="6"/>
+      <c r="A1099" s="4"/>
+      <c r="B1099" s="5"/>
     </row>
     <row r="1100" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1100" s="5"/>
-      <c r="B1100" s="6"/>
+      <c r="A1100" s="4"/>
+      <c r="B1100" s="5"/>
     </row>
     <row r="1101" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1101" s="5"/>
-      <c r="B1101" s="6"/>
+      <c r="A1101" s="4"/>
+      <c r="B1101" s="5"/>
     </row>
     <row r="1102" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1102" s="5"/>
-      <c r="B1102" s="6"/>
+      <c r="A1102" s="4"/>
+      <c r="B1102" s="5"/>
     </row>
     <row r="1103" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1103" s="5"/>
-      <c r="B1103" s="6"/>
+      <c r="A1103" s="4"/>
+      <c r="B1103" s="5"/>
     </row>
     <row r="1104" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1104" s="5"/>
-      <c r="B1104" s="6"/>
+      <c r="A1104" s="4"/>
+      <c r="B1104" s="5"/>
     </row>
     <row r="1105" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1105" s="5"/>
-      <c r="B1105" s="6"/>
+      <c r="A1105" s="4"/>
+      <c r="B1105" s="5"/>
     </row>
     <row r="1106" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1106" s="5"/>
-      <c r="B1106" s="6"/>
+      <c r="A1106" s="4"/>
+      <c r="B1106" s="5"/>
     </row>
     <row r="1107" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1107" s="5"/>
-      <c r="B1107" s="6"/>
+      <c r="A1107" s="4"/>
+      <c r="B1107" s="5"/>
     </row>
     <row r="1108" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1108" s="5"/>
-      <c r="B1108" s="6"/>
+      <c r="A1108" s="4"/>
+      <c r="B1108" s="5"/>
     </row>
     <row r="1109" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1109" s="5"/>
-      <c r="B1109" s="6"/>
+      <c r="A1109" s="4"/>
+      <c r="B1109" s="5"/>
     </row>
     <row r="1110" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1110" s="5"/>
-      <c r="B1110" s="6"/>
+      <c r="A1110" s="4"/>
+      <c r="B1110" s="5"/>
     </row>
     <row r="1111" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1111" s="5"/>
-      <c r="B1111" s="6"/>
+      <c r="A1111" s="4"/>
+      <c r="B1111" s="5"/>
     </row>
     <row r="1112" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1112" s="5"/>
-      <c r="B1112" s="6"/>
+      <c r="A1112" s="4"/>
+      <c r="B1112" s="5"/>
     </row>
     <row r="1113" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1113" s="5"/>
-      <c r="B1113" s="6"/>
+      <c r="A1113" s="4"/>
+      <c r="B1113" s="5"/>
     </row>
     <row r="1114" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1114" s="5"/>
-      <c r="B1114" s="6"/>
+      <c r="A1114" s="4"/>
+      <c r="B1114" s="5"/>
     </row>
     <row r="1115" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1115" s="5"/>
-      <c r="B1115" s="6"/>
+      <c r="A1115" s="4"/>
+      <c r="B1115" s="5"/>
     </row>
     <row r="1116" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1116" s="5"/>
-      <c r="B1116" s="6"/>
+      <c r="A1116" s="4"/>
+      <c r="B1116" s="5"/>
     </row>
     <row r="1117" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1117" s="5"/>
-      <c r="B1117" s="6"/>
+      <c r="A1117" s="4"/>
+      <c r="B1117" s="5"/>
     </row>
     <row r="1118" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1118" s="5"/>
-      <c r="B1118" s="6"/>
+      <c r="A1118" s="4"/>
+      <c r="B1118" s="5"/>
     </row>
     <row r="1119" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1119" s="5"/>
-      <c r="B1119" s="6"/>
+      <c r="A1119" s="4"/>
+      <c r="B1119" s="5"/>
     </row>
     <row r="1120" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1120" s="5"/>
-      <c r="B1120" s="6"/>
+      <c r="A1120" s="4"/>
+      <c r="B1120" s="5"/>
     </row>
     <row r="1121" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1121" s="5"/>
-      <c r="B1121" s="6"/>
+      <c r="A1121" s="4"/>
+      <c r="B1121" s="5"/>
     </row>
     <row r="1122" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1122" s="5"/>
-      <c r="B1122" s="6"/>
+      <c r="A1122" s="4"/>
+      <c r="B1122" s="5"/>
     </row>
     <row r="1123" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1123" s="5"/>
-      <c r="B1123" s="6"/>
+      <c r="A1123" s="4"/>
+      <c r="B1123" s="5"/>
     </row>
     <row r="1124" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1124" s="5"/>
-      <c r="B1124" s="6"/>
+      <c r="A1124" s="4"/>
+      <c r="B1124" s="5"/>
     </row>
     <row r="1125" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1125" s="5"/>
-      <c r="B1125" s="6"/>
+      <c r="A1125" s="4"/>
+      <c r="B1125" s="5"/>
     </row>
     <row r="1126" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1126" s="5"/>
-      <c r="B1126" s="6"/>
+      <c r="A1126" s="4"/>
+      <c r="B1126" s="5"/>
     </row>
     <row r="1127" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1127" s="5"/>
-      <c r="B1127" s="6"/>
+      <c r="A1127" s="4"/>
+      <c r="B1127" s="5"/>
     </row>
     <row r="1128" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1128" s="5"/>
-      <c r="B1128" s="6"/>
+      <c r="A1128" s="4"/>
+      <c r="B1128" s="5"/>
     </row>
     <row r="1129" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1129" s="5"/>
-      <c r="B1129" s="6"/>
+      <c r="A1129" s="4"/>
+      <c r="B1129" s="5"/>
     </row>
     <row r="1130" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1130" s="5"/>
-      <c r="B1130" s="6"/>
+      <c r="A1130" s="4"/>
+      <c r="B1130" s="5"/>
     </row>
     <row r="1131" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1131" s="5"/>
-      <c r="B1131" s="6"/>
+      <c r="A1131" s="4"/>
+      <c r="B1131" s="5"/>
     </row>
     <row r="1132" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1132" s="5"/>
-      <c r="B1132" s="6"/>
+      <c r="A1132" s="4"/>
+      <c r="B1132" s="5"/>
     </row>
     <row r="1133" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1133" s="5"/>
-      <c r="B1133" s="6"/>
+      <c r="A1133" s="4"/>
+      <c r="B1133" s="5"/>
     </row>
     <row r="1134" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1134" s="5"/>
-      <c r="B1134" s="6"/>
+      <c r="A1134" s="4"/>
+      <c r="B1134" s="5"/>
     </row>
     <row r="1135" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1135" s="5"/>
-      <c r="B1135" s="6"/>
+      <c r="A1135" s="4"/>
+      <c r="B1135" s="5"/>
     </row>
     <row r="1136" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1136" s="5"/>
-      <c r="B1136" s="6"/>
+      <c r="A1136" s="4"/>
+      <c r="B1136" s="5"/>
     </row>
     <row r="1137" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1137" s="5"/>
-      <c r="B1137" s="6"/>
+      <c r="A1137" s="4"/>
+      <c r="B1137" s="5"/>
     </row>
     <row r="1138" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1138" s="5"/>
-      <c r="B1138" s="6"/>
+      <c r="A1138" s="4"/>
+      <c r="B1138" s="5"/>
     </row>
     <row r="1139" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1139" s="5"/>
-      <c r="B1139" s="6"/>
+      <c r="A1139" s="4"/>
+      <c r="B1139" s="5"/>
     </row>
     <row r="1140" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1140" s="5"/>
-      <c r="B1140" s="6"/>
+      <c r="A1140" s="4"/>
+      <c r="B1140" s="5"/>
     </row>
     <row r="1141" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1141" s="5"/>
-      <c r="B1141" s="6"/>
+      <c r="A1141" s="4"/>
+      <c r="B1141" s="5"/>
     </row>
     <row r="1142" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1142" s="5"/>
-      <c r="B1142" s="6"/>
+      <c r="A1142" s="4"/>
+      <c r="B1142" s="5"/>
     </row>
     <row r="1143" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1143" s="5"/>
-      <c r="B1143" s="6"/>
+      <c r="A1143" s="4"/>
+      <c r="B1143" s="5"/>
     </row>
     <row r="1144" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1144" s="5"/>
-      <c r="B1144" s="6"/>
+      <c r="A1144" s="4"/>
+      <c r="B1144" s="5"/>
     </row>
     <row r="1145" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1145" s="5"/>
-      <c r="B1145" s="6"/>
+      <c r="A1145" s="4"/>
+      <c r="B1145" s="5"/>
     </row>
     <row r="1146" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1146" s="5"/>
-      <c r="B1146" s="6"/>
+      <c r="A1146" s="4"/>
+      <c r="B1146" s="5"/>
     </row>
     <row r="1147" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1147" s="5"/>
-      <c r="B1147" s="6"/>
+      <c r="A1147" s="4"/>
+      <c r="B1147" s="5"/>
     </row>
     <row r="1148" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1148" s="5"/>
-      <c r="B1148" s="6"/>
+      <c r="A1148" s="4"/>
+      <c r="B1148" s="5"/>
     </row>
     <row r="1149" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1149" s="5"/>
-      <c r="B1149" s="6"/>
+      <c r="A1149" s="4"/>
+      <c r="B1149" s="5"/>
     </row>
     <row r="1150" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1150" s="5"/>
-      <c r="B1150" s="6"/>
+      <c r="A1150" s="4"/>
+      <c r="B1150" s="5"/>
     </row>
     <row r="1151" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1151" s="5"/>
-      <c r="B1151" s="6"/>
+      <c r="A1151" s="4"/>
+      <c r="B1151" s="5"/>
     </row>
     <row r="1152" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1152" s="5"/>
-      <c r="B1152" s="6"/>
+      <c r="A1152" s="4"/>
+      <c r="B1152" s="5"/>
     </row>
     <row r="1153" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1153" s="5"/>
-      <c r="B1153" s="6"/>
+      <c r="A1153" s="4"/>
+      <c r="B1153" s="5"/>
     </row>
     <row r="1154" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1154" s="5"/>
-      <c r="B1154" s="6"/>
+      <c r="A1154" s="4"/>
+      <c r="B1154" s="5"/>
     </row>
     <row r="1155" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1155" s="5"/>
-      <c r="B1155" s="6"/>
+      <c r="A1155" s="4"/>
+      <c r="B1155" s="5"/>
     </row>
     <row r="1156" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1156" s="5"/>
-      <c r="B1156" s="6"/>
+      <c r="A1156" s="4"/>
+      <c r="B1156" s="5"/>
     </row>
     <row r="1157" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1157" s="5"/>
-      <c r="B1157" s="6"/>
+      <c r="A1157" s="4"/>
+      <c r="B1157" s="5"/>
     </row>
     <row r="1158" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1158" s="5"/>
-      <c r="B1158" s="6"/>
+      <c r="A1158" s="4"/>
+      <c r="B1158" s="5"/>
     </row>
     <row r="1159" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1159" s="5"/>
-      <c r="B1159" s="6"/>
+      <c r="A1159" s="4"/>
+      <c r="B1159" s="5"/>
     </row>
     <row r="1160" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1160" s="5"/>
-      <c r="B1160" s="6"/>
+      <c r="A1160" s="4"/>
+      <c r="B1160" s="5"/>
     </row>
     <row r="1161" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1161" s="5"/>
-      <c r="B1161" s="6"/>
+      <c r="A1161" s="4"/>
+      <c r="B1161" s="5"/>
     </row>
     <row r="1162" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1162" s="5"/>
-      <c r="B1162" s="6"/>
+      <c r="A1162" s="4"/>
+      <c r="B1162" s="5"/>
     </row>
     <row r="1163" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1163" s="5"/>
-      <c r="B1163" s="6"/>
+      <c r="A1163" s="4"/>
+      <c r="B1163" s="5"/>
     </row>
     <row r="1164" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1164" s="5"/>
-      <c r="B1164" s="6"/>
+      <c r="A1164" s="4"/>
+      <c r="B1164" s="5"/>
     </row>
     <row r="1165" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1165" s="5"/>
-      <c r="B1165" s="6"/>
+      <c r="A1165" s="4"/>
+      <c r="B1165" s="5"/>
     </row>
     <row r="1166" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1166" s="5"/>
-      <c r="B1166" s="6"/>
+      <c r="A1166" s="4"/>
+      <c r="B1166" s="5"/>
     </row>
     <row r="1167" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1167" s="5"/>
-      <c r="B1167" s="6"/>
+      <c r="A1167" s="4"/>
+      <c r="B1167" s="5"/>
     </row>
     <row r="1168" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1168" s="5"/>
-      <c r="B1168" s="6"/>
+      <c r="A1168" s="4"/>
+      <c r="B1168" s="5"/>
     </row>
     <row r="1169" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1169" s="5"/>
-      <c r="B1169" s="6"/>
+      <c r="A1169" s="4"/>
+      <c r="B1169" s="5"/>
     </row>
     <row r="1170" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1170" s="5"/>
-      <c r="B1170" s="6"/>
+      <c r="A1170" s="4"/>
+      <c r="B1170" s="5"/>
     </row>
     <row r="1171" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1171" s="5"/>
-      <c r="B1171" s="6"/>
+      <c r="A1171" s="4"/>
+      <c r="B1171" s="5"/>
     </row>
     <row r="1172" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1172" s="5"/>
-      <c r="B1172" s="6"/>
+      <c r="A1172" s="4"/>
+      <c r="B1172" s="5"/>
     </row>
     <row r="1173" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1173" s="5"/>
-      <c r="B1173" s="6"/>
+      <c r="A1173" s="4"/>
+      <c r="B1173" s="5"/>
     </row>
     <row r="1174" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1174" s="5"/>
-      <c r="B1174" s="6"/>
+      <c r="A1174" s="4"/>
+      <c r="B1174" s="5"/>
     </row>
     <row r="1175" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1175" s="5"/>
-      <c r="B1175" s="6"/>
+      <c r="A1175" s="4"/>
+      <c r="B1175" s="5"/>
     </row>
     <row r="1176" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1176" s="5"/>
-      <c r="B1176" s="6"/>
+      <c r="A1176" s="4"/>
+      <c r="B1176" s="5"/>
     </row>
     <row r="1177" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1177" s="5"/>
-      <c r="B1177" s="6"/>
+      <c r="A1177" s="4"/>
+      <c r="B1177" s="5"/>
     </row>
     <row r="1178" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1178" s="5"/>
-      <c r="B1178" s="6"/>
+      <c r="A1178" s="4"/>
+      <c r="B1178" s="5"/>
     </row>
     <row r="1179" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1179" s="5"/>
-      <c r="B1179" s="6"/>
+      <c r="A1179" s="4"/>
+      <c r="B1179" s="5"/>
     </row>
     <row r="1180" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1180" s="5"/>
-      <c r="B1180" s="6"/>
+      <c r="A1180" s="4"/>
+      <c r="B1180" s="5"/>
     </row>
     <row r="1181" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1181" s="5"/>
-      <c r="B1181" s="6"/>
+      <c r="A1181" s="4"/>
+      <c r="B1181" s="5"/>
     </row>
     <row r="1182" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1182" s="5"/>
-      <c r="B1182" s="6"/>
+      <c r="A1182" s="4"/>
+      <c r="B1182" s="5"/>
     </row>
     <row r="1183" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1183" s="5"/>
-      <c r="B1183" s="6"/>
+      <c r="A1183" s="4"/>
+      <c r="B1183" s="5"/>
     </row>
     <row r="1184" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1184" s="5"/>
-      <c r="B1184" s="6"/>
+      <c r="A1184" s="4"/>
+      <c r="B1184" s="5"/>
     </row>
     <row r="1185" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1185" s="5"/>
-      <c r="B1185" s="6"/>
+      <c r="A1185" s="4"/>
+      <c r="B1185" s="5"/>
     </row>
     <row r="1186" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1186" s="5"/>
-      <c r="B1186" s="6"/>
+      <c r="A1186" s="4"/>
+      <c r="B1186" s="5"/>
     </row>
     <row r="1187" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1187" s="5"/>
-      <c r="B1187" s="6"/>
+      <c r="A1187" s="4"/>
+      <c r="B1187" s="5"/>
     </row>
     <row r="1188" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1188" s="5"/>
-      <c r="B1188" s="6"/>
+      <c r="A1188" s="4"/>
+      <c r="B1188" s="5"/>
     </row>
     <row r="1189" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1189" s="5"/>
-      <c r="B1189" s="6"/>
+      <c r="A1189" s="4"/>
+      <c r="B1189" s="5"/>
     </row>
     <row r="1190" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1190" s="5"/>
-      <c r="B1190" s="6"/>
+      <c r="A1190" s="4"/>
+      <c r="B1190" s="5"/>
     </row>
     <row r="1191" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1191" s="5"/>
-      <c r="B1191" s="6"/>
+      <c r="A1191" s="4"/>
+      <c r="B1191" s="5"/>
     </row>
     <row r="1192" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1192" s="5"/>
-      <c r="B1192" s="6"/>
+      <c r="A1192" s="4"/>
+      <c r="B1192" s="5"/>
     </row>
     <row r="1193" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1193" s="5"/>
-      <c r="B1193" s="6"/>
+      <c r="A1193" s="4"/>
+      <c r="B1193" s="5"/>
     </row>
     <row r="1194" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1194" s="5"/>
-      <c r="B1194" s="6"/>
+      <c r="A1194" s="4"/>
+      <c r="B1194" s="5"/>
     </row>
     <row r="1195" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1195" s="5"/>
-      <c r="B1195" s="6"/>
+      <c r="A1195" s="4"/>
+      <c r="B1195" s="5"/>
     </row>
     <row r="1196" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1196" s="5"/>
-      <c r="B1196" s="6"/>
+      <c r="A1196" s="4"/>
+      <c r="B1196" s="5"/>
     </row>
     <row r="1197" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1197" s="5"/>
-      <c r="B1197" s="6"/>
+      <c r="A1197" s="4"/>
+      <c r="B1197" s="5"/>
     </row>
     <row r="1198" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1198" s="5"/>
-      <c r="B1198" s="6"/>
+      <c r="A1198" s="4"/>
+      <c r="B1198" s="5"/>
     </row>
     <row r="1199" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1199" s="5"/>
-      <c r="B1199" s="6"/>
+      <c r="A1199" s="4"/>
+      <c r="B1199" s="5"/>
     </row>
     <row r="1200" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1200" s="5"/>
-      <c r="B1200" s="6"/>
+      <c r="A1200" s="4"/>
+      <c r="B1200" s="5"/>
     </row>
     <row r="1201" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1201" s="5"/>
-      <c r="B1201" s="6"/>
+      <c r="A1201" s="4"/>
+      <c r="B1201" s="5"/>
     </row>
     <row r="1202" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1202" s="5"/>
-      <c r="B1202" s="6"/>
+      <c r="A1202" s="4"/>
+      <c r="B1202" s="5"/>
     </row>
     <row r="1203" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1203" s="5"/>
-      <c r="B1203" s="6"/>
+      <c r="A1203" s="4"/>
+      <c r="B1203" s="5"/>
     </row>
     <row r="1204" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1204" s="5"/>
-      <c r="B1204" s="6"/>
+      <c r="A1204" s="4"/>
+      <c r="B1204" s="5"/>
     </row>
     <row r="1205" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1205" s="5"/>
-      <c r="B1205" s="6"/>
+      <c r="A1205" s="4"/>
+      <c r="B1205" s="5"/>
     </row>
     <row r="1206" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1206" s="5"/>
-      <c r="B1206" s="6"/>
+      <c r="A1206" s="4"/>
+      <c r="B1206" s="5"/>
     </row>
     <row r="1207" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1207" s="5"/>
-      <c r="B1207" s="6"/>
+      <c r="A1207" s="4"/>
+      <c r="B1207" s="5"/>
     </row>
     <row r="1208" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1208" s="5"/>
-      <c r="B1208" s="6"/>
+      <c r="A1208" s="4"/>
+      <c r="B1208" s="5"/>
     </row>
     <row r="1209" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1209" s="5"/>
-      <c r="B1209" s="6"/>
+      <c r="A1209" s="4"/>
+      <c r="B1209" s="5"/>
     </row>
     <row r="1210" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1210" s="5"/>
-      <c r="B1210" s="6"/>
+      <c r="A1210" s="4"/>
+      <c r="B1210" s="5"/>
     </row>
     <row r="1211" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1211" s="5"/>
-      <c r="B1211" s="6"/>
+      <c r="A1211" s="4"/>
+      <c r="B1211" s="5"/>
     </row>
     <row r="1212" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1212" s="5"/>
-      <c r="B1212" s="6"/>
+      <c r="A1212" s="4"/>
+      <c r="B1212" s="5"/>
     </row>
     <row r="1213" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1213" s="5"/>
-      <c r="B1213" s="6"/>
+      <c r="A1213" s="4"/>
+      <c r="B1213" s="5"/>
     </row>
     <row r="1214" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1214" s="5"/>
-      <c r="B1214" s="6"/>
+      <c r="A1214" s="4"/>
+      <c r="B1214" s="5"/>
     </row>
     <row r="1215" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1215" s="5"/>
-      <c r="B1215" s="6"/>
+      <c r="A1215" s="4"/>
+      <c r="B1215" s="5"/>
     </row>
     <row r="1216" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1216" s="5"/>
-      <c r="B1216" s="6"/>
+      <c r="A1216" s="4"/>
+      <c r="B1216" s="5"/>
     </row>
     <row r="1217" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1217" s="5"/>
-      <c r="B1217" s="6"/>
+      <c r="A1217" s="4"/>
+      <c r="B1217" s="5"/>
     </row>
     <row r="1218" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1218" s="5"/>
-      <c r="B1218" s="6"/>
+      <c r="A1218" s="4"/>
+      <c r="B1218" s="5"/>
     </row>
     <row r="1219" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1219" s="5"/>
-      <c r="B1219" s="6"/>
+      <c r="A1219" s="4"/>
+      <c r="B1219" s="5"/>
     </row>
     <row r="1220" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1220" s="5"/>
-      <c r="B1220" s="6"/>
+      <c r="A1220" s="4"/>
+      <c r="B1220" s="5"/>
     </row>
     <row r="1221" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1221" s="5"/>
-      <c r="B1221" s="6"/>
+      <c r="A1221" s="4"/>
+      <c r="B1221" s="5"/>
     </row>
     <row r="1222" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1222" s="5"/>
-      <c r="B1222" s="6"/>
+      <c r="A1222" s="4"/>
+      <c r="B1222" s="5"/>
     </row>
     <row r="1223" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1223" s="5"/>
-      <c r="B1223" s="6"/>
+      <c r="A1223" s="4"/>
+      <c r="B1223" s="5"/>
     </row>
     <row r="1224" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1224" s="5"/>
-      <c r="B1224" s="6"/>
+      <c r="A1224" s="4"/>
+      <c r="B1224" s="5"/>
     </row>
     <row r="1225" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1225" s="5"/>
-      <c r="B1225" s="6"/>
+      <c r="A1225" s="4"/>
+      <c r="B1225" s="5"/>
     </row>
     <row r="1226" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1226" s="5"/>
-      <c r="B1226" s="6"/>
+      <c r="A1226" s="4"/>
+      <c r="B1226" s="5"/>
     </row>
     <row r="1227" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1227" s="5"/>
-      <c r="B1227" s="6"/>
+      <c r="A1227" s="4"/>
+      <c r="B1227" s="5"/>
     </row>
     <row r="1228" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1228" s="5"/>
-      <c r="B1228" s="6"/>
+      <c r="A1228" s="4"/>
+      <c r="B1228" s="5"/>
     </row>
     <row r="1229" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1229" s="5"/>
-      <c r="B1229" s="6"/>
+      <c r="A1229" s="4"/>
+      <c r="B1229" s="5"/>
     </row>
     <row r="1230" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1230" s="5"/>
-      <c r="B1230" s="6"/>
+      <c r="A1230" s="4"/>
+      <c r="B1230" s="5"/>
     </row>
     <row r="1231" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1231" s="5"/>
-      <c r="B1231" s="6"/>
+      <c r="A1231" s="4"/>
+      <c r="B1231" s="5"/>
     </row>
     <row r="1232" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1232" s="5"/>
-      <c r="B1232" s="6"/>
+      <c r="A1232" s="4"/>
+      <c r="B1232" s="5"/>
     </row>
     <row r="1233" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1233" s="5"/>
-      <c r="B1233" s="6"/>
+      <c r="A1233" s="4"/>
+      <c r="B1233" s="5"/>
     </row>
     <row r="1234" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1234" s="5"/>
-      <c r="B1234" s="6"/>
+      <c r="A1234" s="4"/>
+      <c r="B1234" s="5"/>
     </row>
     <row r="1235" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1235" s="5"/>
-      <c r="B1235" s="6"/>
+      <c r="A1235" s="4"/>
+      <c r="B1235" s="5"/>
     </row>
     <row r="1236" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1236" s="5"/>
-      <c r="B1236" s="6"/>
+      <c r="A1236" s="4"/>
+      <c r="B1236" s="5"/>
     </row>
     <row r="1237" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1237" s="5"/>
-      <c r="B1237" s="6"/>
+      <c r="A1237" s="4"/>
+      <c r="B1237" s="5"/>
     </row>
     <row r="1238" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1238" s="5"/>
-      <c r="B1238" s="6"/>
+      <c r="A1238" s="4"/>
+      <c r="B1238" s="5"/>
     </row>
     <row r="1239" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1239" s="5"/>
-      <c r="B1239" s="6"/>
+      <c r="A1239" s="4"/>
+      <c r="B1239" s="5"/>
     </row>
     <row r="1240" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1240" s="5"/>
-      <c r="B1240" s="6"/>
+      <c r="A1240" s="4"/>
+      <c r="B1240" s="5"/>
     </row>
     <row r="1241" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1241" s="5"/>
-      <c r="B1241" s="6"/>
+      <c r="A1241" s="4"/>
+      <c r="B1241" s="5"/>
     </row>
     <row r="1242" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1242" s="5"/>
-      <c r="B1242" s="6"/>
+      <c r="A1242" s="4"/>
+      <c r="B1242" s="5"/>
     </row>
     <row r="1243" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1243" s="5"/>
-      <c r="B1243" s="6"/>
+      <c r="A1243" s="4"/>
+      <c r="B1243" s="5"/>
     </row>
     <row r="1244" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1244" s="5"/>
-      <c r="B1244" s="6"/>
+      <c r="A1244" s="4"/>
+      <c r="B1244" s="5"/>
     </row>
     <row r="1245" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1245" s="5"/>
-      <c r="B1245" s="6"/>
+      <c r="A1245" s="4"/>
+      <c r="B1245" s="5"/>
     </row>
     <row r="1246" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1246" s="5"/>
-      <c r="B1246" s="6"/>
+      <c r="A1246" s="4"/>
+      <c r="B1246" s="5"/>
     </row>
     <row r="1247" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1247" s="5"/>
-      <c r="B1247" s="6"/>
+      <c r="A1247" s="4"/>
+      <c r="B1247" s="5"/>
     </row>
     <row r="1248" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1248" s="5"/>
-      <c r="B1248" s="6"/>
+      <c r="A1248" s="4"/>
+      <c r="B1248" s="5"/>
     </row>
     <row r="1249" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1249" s="5"/>
-      <c r="B1249" s="6"/>
+      <c r="A1249" s="4"/>
+      <c r="B1249" s="5"/>
     </row>
     <row r="1250" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1250" s="5"/>
-      <c r="B1250" s="6"/>
+      <c r="A1250" s="4"/>
+      <c r="B1250" s="5"/>
     </row>
     <row r="1251" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1251" s="5"/>
-      <c r="B1251" s="6"/>
+      <c r="A1251" s="4"/>
+      <c r="B1251" s="5"/>
     </row>
     <row r="1252" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1252" s="5"/>
-      <c r="B1252" s="6"/>
+      <c r="A1252" s="4"/>
+      <c r="B1252" s="5"/>
     </row>
     <row r="1253" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1253" s="5"/>
-      <c r="B1253" s="6"/>
+      <c r="A1253" s="4"/>
+      <c r="B1253" s="5"/>
     </row>
     <row r="1254" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1254" s="5"/>
-      <c r="B1254" s="6"/>
+      <c r="A1254" s="4"/>
+      <c r="B1254" s="5"/>
     </row>
     <row r="1255" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1255" s="5"/>
-      <c r="B1255" s="6"/>
+      <c r="A1255" s="4"/>
+      <c r="B1255" s="5"/>
     </row>
     <row r="1256" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1256" s="5"/>
-      <c r="B1256" s="6"/>
+      <c r="A1256" s="4"/>
+      <c r="B1256" s="5"/>
     </row>
     <row r="1257" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1257" s="5"/>
-      <c r="B1257" s="6"/>
+      <c r="A1257" s="4"/>
+      <c r="B1257" s="5"/>
     </row>
     <row r="1258" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1258" s="5"/>
-      <c r="B1258" s="6"/>
+      <c r="A1258" s="4"/>
+      <c r="B1258" s="5"/>
     </row>
     <row r="1259" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1259" s="5"/>
-      <c r="B1259" s="6"/>
+      <c r="A1259" s="4"/>
+      <c r="B1259" s="5"/>
     </row>
     <row r="1260" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1260" s="5"/>
-      <c r="B1260" s="6"/>
+      <c r="A1260" s="4"/>
+      <c r="B1260" s="5"/>
     </row>
     <row r="1261" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1261" s="5"/>
-      <c r="B1261" s="6"/>
+      <c r="A1261" s="4"/>
+      <c r="B1261" s="5"/>
     </row>
     <row r="1262" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1262" s="5"/>
-      <c r="B1262" s="6"/>
+      <c r="A1262" s="4"/>
+      <c r="B1262" s="5"/>
     </row>
     <row r="1263" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1263" s="5"/>
-      <c r="B1263" s="6"/>
+      <c r="A1263" s="4"/>
+      <c r="B1263" s="5"/>
     </row>
     <row r="1264" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1264" s="5"/>
-      <c r="B1264" s="6"/>
+      <c r="A1264" s="4"/>
+      <c r="B1264" s="5"/>
     </row>
     <row r="1265" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1265" s="5"/>
-      <c r="B1265" s="6"/>
+      <c r="A1265" s="4"/>
+      <c r="B1265" s="5"/>
     </row>
     <row r="1266" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1266" s="5"/>
-      <c r="B1266" s="6"/>
+      <c r="A1266" s="4"/>
+      <c r="B1266" s="5"/>
     </row>
     <row r="1267" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1267" s="5"/>
-      <c r="B1267" s="6"/>
+      <c r="A1267" s="4"/>
+      <c r="B1267" s="5"/>
     </row>
     <row r="1268" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1268" s="5"/>
-      <c r="B1268" s="6"/>
+      <c r="A1268" s="4"/>
+      <c r="B1268" s="5"/>
     </row>
     <row r="1269" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1269" s="5"/>
-      <c r="B1269" s="6"/>
+      <c r="A1269" s="4"/>
+      <c r="B1269" s="5"/>
     </row>
     <row r="1270" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1270" s="5"/>
-      <c r="B1270" s="6"/>
+      <c r="A1270" s="4"/>
+      <c r="B1270" s="5"/>
     </row>
     <row r="1271" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1271" s="5"/>
-      <c r="B1271" s="6"/>
+      <c r="A1271" s="4"/>
+      <c r="B1271" s="5"/>
     </row>
     <row r="1272" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1272" s="5"/>
-      <c r="B1272" s="6"/>
+      <c r="A1272" s="4"/>
+      <c r="B1272" s="5"/>
     </row>
     <row r="1273" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1273" s="5"/>
-      <c r="B1273" s="6"/>
+      <c r="A1273" s="4"/>
+      <c r="B1273" s="5"/>
     </row>
     <row r="1274" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1274" s="5"/>
-      <c r="B1274" s="6"/>
+      <c r="A1274" s="4"/>
+      <c r="B1274" s="5"/>
     </row>
     <row r="1275" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1275" s="5"/>
-      <c r="B1275" s="6"/>
+      <c r="A1275" s="4"/>
+      <c r="B1275" s="5"/>
     </row>
     <row r="1276" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1276" s="5"/>
-      <c r="B1276" s="6"/>
+      <c r="A1276" s="4"/>
+      <c r="B1276" s="5"/>
     </row>
     <row r="1277" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1277" s="5"/>
-      <c r="B1277" s="6"/>
+      <c r="A1277" s="4"/>
+      <c r="B1277" s="5"/>
     </row>
     <row r="1278" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1278" s="5"/>
-      <c r="B1278" s="6"/>
+      <c r="A1278" s="4"/>
+      <c r="B1278" s="5"/>
     </row>
     <row r="1279" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1279" s="5"/>
-      <c r="B1279" s="6"/>
+      <c r="A1279" s="4"/>
+      <c r="B1279" s="5"/>
     </row>
     <row r="1280" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1280" s="5"/>
-      <c r="B1280" s="6"/>
+      <c r="A1280" s="4"/>
+      <c r="B1280" s="5"/>
     </row>
     <row r="1281" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1281" s="5"/>
-      <c r="B1281" s="6"/>
+      <c r="A1281" s="4"/>
+      <c r="B1281" s="5"/>
     </row>
     <row r="1282" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1282" s="5"/>
-      <c r="B1282" s="6"/>
+      <c r="A1282" s="4"/>
+      <c r="B1282" s="5"/>
     </row>
     <row r="1283" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1283" s="5"/>
-      <c r="B1283" s="6"/>
+      <c r="A1283" s="4"/>
+      <c r="B1283" s="5"/>
     </row>
     <row r="1284" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1284" s="5"/>
-      <c r="B1284" s="6"/>
+      <c r="A1284" s="4"/>
+      <c r="B1284" s="5"/>
     </row>
     <row r="1285" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1285" s="5"/>
-      <c r="B1285" s="6"/>
+      <c r="A1285" s="4"/>
+      <c r="B1285" s="5"/>
     </row>
     <row r="1286" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1286" s="5"/>
-      <c r="B1286" s="6"/>
+      <c r="A1286" s="4"/>
+      <c r="B1286" s="5"/>
     </row>
     <row r="1287" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1287" s="5"/>
-      <c r="B1287" s="6"/>
+      <c r="A1287" s="4"/>
+      <c r="B1287" s="5"/>
     </row>
     <row r="1288" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1288" s="5"/>
-      <c r="B1288" s="6"/>
+      <c r="A1288" s="4"/>
+      <c r="B1288" s="5"/>
     </row>
     <row r="1289" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1289" s="5"/>
-      <c r="B1289" s="6"/>
+      <c r="A1289" s="4"/>
+      <c r="B1289" s="5"/>
     </row>
     <row r="1290" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1290" s="5"/>
-      <c r="B1290" s="6"/>
+      <c r="A1290" s="4"/>
+      <c r="B1290" s="5"/>
     </row>
     <row r="1291" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1291" s="5"/>
-      <c r="B1291" s="6"/>
+      <c r="A1291" s="4"/>
+      <c r="B1291" s="5"/>
     </row>
     <row r="1292" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1292" s="5"/>
-      <c r="B1292" s="6"/>
+      <c r="A1292" s="4"/>
+      <c r="B1292" s="5"/>
     </row>
     <row r="1293" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1293" s="5"/>
-      <c r="B1293" s="6"/>
+      <c r="A1293" s="4"/>
+      <c r="B1293" s="5"/>
     </row>
     <row r="1294" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1294" s="5"/>
-      <c r="B1294" s="6"/>
+      <c r="A1294" s="4"/>
+      <c r="B1294" s="5"/>
     </row>
     <row r="1295" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1295" s="5"/>
-      <c r="B1295" s="6"/>
+      <c r="A1295" s="4"/>
+      <c r="B1295" s="5"/>
     </row>
     <row r="1296" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1296" s="5"/>
-      <c r="B1296" s="6"/>
+      <c r="A1296" s="4"/>
+      <c r="B1296" s="5"/>
     </row>
     <row r="1297" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1297" s="5"/>
-      <c r="B1297" s="6"/>
+      <c r="A1297" s="4"/>
+      <c r="B1297" s="5"/>
     </row>
     <row r="1298" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1298" s="5"/>
-      <c r="B1298" s="6"/>
+      <c r="A1298" s="4"/>
+      <c r="B1298" s="5"/>
     </row>
     <row r="1299" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1299" s="5"/>
-      <c r="B1299" s="6"/>
+      <c r="A1299" s="4"/>
+      <c r="B1299" s="5"/>
     </row>
     <row r="1300" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1300" s="5"/>
-      <c r="B1300" s="6"/>
+      <c r="A1300" s="4"/>
+      <c r="B1300" s="5"/>
     </row>
     <row r="1301" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1301" s="5"/>
-      <c r="B1301" s="6"/>
+      <c r="A1301" s="4"/>
+      <c r="B1301" s="5"/>
     </row>
     <row r="1302" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1302" s="5"/>
-      <c r="B1302" s="6"/>
+      <c r="A1302" s="4"/>
+      <c r="B1302" s="5"/>
     </row>
     <row r="1303" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1303" s="5"/>
-      <c r="B1303" s="6"/>
+      <c r="A1303" s="4"/>
+      <c r="B1303" s="5"/>
     </row>
     <row r="1304" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1304" s="5"/>
-      <c r="B1304" s="6"/>
+      <c r="A1304" s="4"/>
+      <c r="B1304" s="5"/>
     </row>
     <row r="1305" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1305" s="5"/>
-      <c r="B1305" s="6"/>
+      <c r="A1305" s="4"/>
+      <c r="B1305" s="5"/>
     </row>
     <row r="1306" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1306" s="5"/>
-      <c r="B1306" s="6"/>
+      <c r="A1306" s="4"/>
+      <c r="B1306" s="5"/>
     </row>
     <row r="1307" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1307" s="5"/>
-      <c r="B1307" s="6"/>
+      <c r="A1307" s="4"/>
+      <c r="B1307" s="5"/>
     </row>
     <row r="1308" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1308" s="5"/>
-      <c r="B1308" s="6"/>
+      <c r="A1308" s="4"/>
+      <c r="B1308" s="5"/>
     </row>
     <row r="1309" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1309" s="5"/>
-      <c r="B1309" s="6"/>
+      <c r="A1309" s="4"/>
+      <c r="B1309" s="5"/>
     </row>
     <row r="1310" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1310" s="5"/>
-      <c r="B1310" s="6"/>
+      <c r="A1310" s="4"/>
+      <c r="B1310" s="5"/>
     </row>
     <row r="1311" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1311" s="5"/>
-      <c r="B1311" s="6"/>
+      <c r="A1311" s="4"/>
+      <c r="B1311" s="5"/>
     </row>
     <row r="1312" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1312" s="5"/>
-      <c r="B1312" s="6"/>
+      <c r="A1312" s="4"/>
+      <c r="B1312" s="5"/>
     </row>
     <row r="1313" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1313" s="5"/>
-      <c r="B1313" s="6"/>
+      <c r="A1313" s="4"/>
+      <c r="B1313" s="5"/>
     </row>
     <row r="1314" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1314" s="5"/>
-      <c r="B1314" s="6"/>
+      <c r="A1314" s="4"/>
+      <c r="B1314" s="5"/>
     </row>
     <row r="1315" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1315" s="5"/>
-      <c r="B1315" s="6"/>
+      <c r="A1315" s="4"/>
+      <c r="B1315" s="5"/>
     </row>
     <row r="1316" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1316" s="5"/>
-      <c r="B1316" s="6"/>
+      <c r="A1316" s="4"/>
+      <c r="B1316" s="5"/>
     </row>
     <row r="1317" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1317" s="5"/>
-      <c r="B1317" s="6"/>
+      <c r="A1317" s="4"/>
+      <c r="B1317" s="5"/>
     </row>
     <row r="1318" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1318" s="5"/>
-      <c r="B1318" s="6"/>
+      <c r="A1318" s="4"/>
+      <c r="B1318" s="5"/>
     </row>
     <row r="1319" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1319" s="5"/>
-      <c r="B1319" s="6"/>
+      <c r="A1319" s="4"/>
+      <c r="B1319" s="5"/>
     </row>
     <row r="1320" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1320" s="5"/>
-      <c r="B1320" s="6"/>
+      <c r="A1320" s="4"/>
+      <c r="B1320" s="5"/>
     </row>
     <row r="1321" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1321" s="5"/>
-      <c r="B1321" s="6"/>
+      <c r="A1321" s="4"/>
+      <c r="B1321" s="5"/>
     </row>
     <row r="1322" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1322" s="5"/>
-      <c r="B1322" s="6"/>
+      <c r="A1322" s="4"/>
+      <c r="B1322" s="5"/>
     </row>
     <row r="1323" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1323" s="5"/>
-      <c r="B1323" s="6"/>
+      <c r="A1323" s="4"/>
+      <c r="B1323" s="5"/>
     </row>
     <row r="1324" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1324" s="5"/>
-      <c r="B1324" s="6"/>
+      <c r="A1324" s="4"/>
+      <c r="B1324" s="5"/>
     </row>
     <row r="1325" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1325" s="5"/>
-      <c r="B1325" s="6"/>
+      <c r="A1325" s="4"/>
+      <c r="B1325" s="5"/>
     </row>
     <row r="1326" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1326" s="5"/>
-      <c r="B1326" s="6"/>
+      <c r="A1326" s="4"/>
+      <c r="B1326" s="5"/>
     </row>
     <row r="1327" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1327" s="5"/>
-      <c r="B1327" s="6"/>
+      <c r="A1327" s="4"/>
+      <c r="B1327" s="5"/>
     </row>
     <row r="1328" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1328" s="5"/>
-      <c r="B1328" s="6"/>
+      <c r="A1328" s="4"/>
+      <c r="B1328" s="5"/>
     </row>
     <row r="1329" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1329" s="5"/>
-      <c r="B1329" s="6"/>
+      <c r="A1329" s="4"/>
+      <c r="B1329" s="5"/>
     </row>
     <row r="1330" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1330" s="5"/>
-      <c r="B1330" s="6"/>
+      <c r="A1330" s="4"/>
+      <c r="B1330" s="5"/>
     </row>
     <row r="1331" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1331" s="5"/>
-      <c r="B1331" s="6"/>
+      <c r="A1331" s="4"/>
+      <c r="B1331" s="5"/>
     </row>
     <row r="1332" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1332" s="5"/>
-      <c r="B1332" s="6"/>
+      <c r="A1332" s="4"/>
+      <c r="B1332" s="5"/>
     </row>
     <row r="1333" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1333" s="5"/>
-      <c r="B1333" s="6"/>
+      <c r="A1333" s="4"/>
+      <c r="B1333" s="5"/>
     </row>
     <row r="1334" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1334" s="5"/>
-      <c r="B1334" s="6"/>
+      <c r="A1334" s="4"/>
+      <c r="B1334" s="5"/>
     </row>
     <row r="1335" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1335" s="5"/>
-      <c r="B1335" s="6"/>
+      <c r="A1335" s="4"/>
+      <c r="B1335" s="5"/>
     </row>
     <row r="1336" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1336" s="5"/>
-      <c r="B1336" s="6"/>
+      <c r="A1336" s="4"/>
+      <c r="B1336" s="5"/>
     </row>
     <row r="1337" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1337" s="5"/>
-      <c r="B1337" s="6"/>
+      <c r="A1337" s="4"/>
+      <c r="B1337" s="5"/>
     </row>
     <row r="1338" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1338" s="5"/>
-      <c r="B1338" s="6"/>
+      <c r="A1338" s="4"/>
+      <c r="B1338" s="5"/>
     </row>
     <row r="1339" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1339" s="5"/>
-      <c r="B1339" s="6"/>
+      <c r="A1339" s="4"/>
+      <c r="B1339" s="5"/>
     </row>
     <row r="1340" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1340" s="5"/>
-      <c r="B1340" s="6"/>
+      <c r="A1340" s="4"/>
+      <c r="B1340" s="5"/>
     </row>
     <row r="1341" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1341" s="5"/>
-      <c r="B1341" s="6"/>
+      <c r="A1341" s="4"/>
+      <c r="B1341" s="5"/>
     </row>
     <row r="1342" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1342" s="5"/>
-      <c r="B1342" s="6"/>
+      <c r="A1342" s="4"/>
+      <c r="B1342" s="5"/>
     </row>
     <row r="1343" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1343" s="5"/>
-      <c r="B1343" s="6"/>
+      <c r="A1343" s="4"/>
+      <c r="B1343" s="5"/>
     </row>
     <row r="1344" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1344" s="5"/>
-      <c r="B1344" s="6"/>
+      <c r="A1344" s="4"/>
+      <c r="B1344" s="5"/>
     </row>
     <row r="1345" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1345" s="5"/>
-      <c r="B1345" s="6"/>
+      <c r="A1345" s="4"/>
+      <c r="B1345" s="5"/>
     </row>
     <row r="1346" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1346" s="5"/>
-      <c r="B1346" s="6"/>
+      <c r="A1346" s="4"/>
+      <c r="B1346" s="5"/>
     </row>
     <row r="1347" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1347" s="5"/>
-      <c r="B1347" s="6"/>
+      <c r="A1347" s="4"/>
+      <c r="B1347" s="5"/>
     </row>
     <row r="1348" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1348" s="5"/>
-      <c r="B1348" s="6"/>
+      <c r="A1348" s="4"/>
+      <c r="B1348" s="5"/>
     </row>
     <row r="1349" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1349" s="5"/>
-      <c r="B1349" s="6"/>
+      <c r="A1349" s="4"/>
+      <c r="B1349" s="5"/>
     </row>
     <row r="1350" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1350" s="5"/>
-      <c r="B1350" s="6"/>
+      <c r="A1350" s="4"/>
+      <c r="B1350" s="5"/>
     </row>
     <row r="1351" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1351" s="5"/>
-      <c r="B1351" s="6"/>
+      <c r="A1351" s="4"/>
+      <c r="B1351" s="5"/>
     </row>
     <row r="1352" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1352" s="5"/>
-      <c r="B1352" s="6"/>
+      <c r="A1352" s="4"/>
+      <c r="B1352" s="5"/>
     </row>
     <row r="1353" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1353" s="8"/>
-      <c r="B1353" s="6"/>
+      <c r="A1353" s="7"/>
+      <c r="B1353" s="5"/>
     </row>
     <row r="1354" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1354" s="8"/>
-      <c r="B1354" s="6"/>
+      <c r="A1354" s="7"/>
+      <c r="B1354" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1">
@@ -25867,215 +25798,215 @@
     <sortCondition ref="D1"/>
   </sortState>
   <conditionalFormatting sqref="E2:E42 E197:E219 E74:E101 E103:E131 E133:E179 E221:E267 E269:E272 E274:E306 E308:E347 E350:E357 E386:E389 E359:E384 E451:E463 E465:E480 E483:E571 E573:E585 E587:E610 E612:E614 E616 E618:E647 E649:E663 E665:E690 E692:E741 E181:E192 E194 E391:E449 E768:E773 E45:E72 E744:E764 E779:E853">
-    <cfRule type="containsText" dxfId="45" priority="43" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="42" priority="43" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E196">
-    <cfRule type="containsText" dxfId="44" priority="42" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="41" priority="42" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E196)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E195">
-    <cfRule type="containsText" dxfId="43" priority="41" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="40" priority="41" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E195)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E73">
-    <cfRule type="containsText" dxfId="42" priority="40" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="39" priority="40" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E102">
-    <cfRule type="containsText" dxfId="41" priority="39" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="38" priority="39" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E102)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E132">
-    <cfRule type="containsText" dxfId="40" priority="38" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="37" priority="38" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E132)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E180">
-    <cfRule type="containsText" dxfId="39" priority="37" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="36" priority="37" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E180)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E220">
-    <cfRule type="containsText" dxfId="38" priority="36" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="35" priority="36" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E220)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E268">
-    <cfRule type="containsText" dxfId="37" priority="35" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="34" priority="35" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E268)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E273">
-    <cfRule type="containsText" dxfId="36" priority="34" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="33" priority="34" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E273)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E307">
-    <cfRule type="containsText" dxfId="35" priority="33" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="32" priority="33" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E307)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E348:E349">
-    <cfRule type="containsText" dxfId="34" priority="32" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="31" priority="32" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E348)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E691">
-    <cfRule type="containsText" dxfId="33" priority="18" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="30" priority="18" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E691)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E358">
-    <cfRule type="containsText" dxfId="32" priority="31" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="29" priority="31" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E358)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E385">
-    <cfRule type="containsText" dxfId="31" priority="30" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="28" priority="30" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E385)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E450">
-    <cfRule type="containsText" dxfId="30" priority="29" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="27" priority="29" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E450)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E464">
-    <cfRule type="containsText" dxfId="29" priority="28" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="26" priority="28" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E464)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E481">
-    <cfRule type="containsText" dxfId="28" priority="27" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="25" priority="27" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E481)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E482">
-    <cfRule type="containsText" dxfId="27" priority="26" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="24" priority="26" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E482)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E572">
-    <cfRule type="containsText" dxfId="26" priority="25" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="23" priority="25" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E572)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E586">
-    <cfRule type="containsText" dxfId="25" priority="24" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="22" priority="24" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E586)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E611">
-    <cfRule type="containsText" dxfId="24" priority="23" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="21" priority="23" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E611)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E615">
-    <cfRule type="containsText" dxfId="23" priority="22" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="20" priority="22" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E615)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E617">
-    <cfRule type="containsText" dxfId="22" priority="21" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="19" priority="21" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E617)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E648">
-    <cfRule type="containsText" dxfId="21" priority="20" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="18" priority="20" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E648)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E664">
-    <cfRule type="containsText" dxfId="20" priority="19" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="17" priority="19" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E664)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E854">
-    <cfRule type="containsText" dxfId="19" priority="17" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="16" priority="17" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E854)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E193">
-    <cfRule type="containsText" dxfId="18" priority="16" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="15" priority="16" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E193)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E390">
-    <cfRule type="containsText" dxfId="17" priority="15" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="14" priority="15" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E390)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="containsText" dxfId="16" priority="14" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="13" priority="14" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="containsText" dxfId="15" priority="13" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="12" priority="13" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E765">
-    <cfRule type="containsText" dxfId="14" priority="12" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="11" priority="12" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E765)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E742">
-    <cfRule type="containsText" dxfId="13" priority="11" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="10" priority="11" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E742)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E743">
-    <cfRule type="containsText" dxfId="12" priority="10" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="9" priority="10" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E743)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E767">
-    <cfRule type="containsText" dxfId="11" priority="9" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="8" priority="9" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E767)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E766">
-    <cfRule type="containsText" dxfId="10" priority="8" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="7" priority="8" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E766)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E776">
-    <cfRule type="containsText" dxfId="9" priority="7" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="6" priority="7" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E776)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E775">
-    <cfRule type="containsText" dxfId="8" priority="6" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="5" priority="6" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E775)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E774">
-    <cfRule type="containsText" dxfId="7" priority="5" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="4" priority="5" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E774)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E778">
-    <cfRule type="containsText" dxfId="6" priority="4" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="3" priority="4" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E778)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E777">
-    <cfRule type="containsText" dxfId="5" priority="3" stopIfTrue="1" operator="containsText" text="grade">
+    <cfRule type="containsText" dxfId="2" priority="3" stopIfTrue="1" operator="containsText" text="grade">
       <formula>NOT(ISERROR(SEARCH("grade",E777)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1">
-    <cfRule type="duplicateValues" dxfId="3" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="45"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://codes.iarc.fr/code/2300"/>
@@ -26860,236 +26791,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId779"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="10.765625" customWidth="1"/>
-    <col min="2" max="2" width="12.765625" customWidth="1"/>
-    <col min="3" max="3" width="24.07421875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15.9" x14ac:dyDescent="0.45">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.9" x14ac:dyDescent="0.45">
-      <c r="A2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2343</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.9" x14ac:dyDescent="0.45">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>2344</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.9" x14ac:dyDescent="0.45">
-      <c r="A4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>2345</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.9" x14ac:dyDescent="0.45">
-      <c r="A5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>2346</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.9" x14ac:dyDescent="0.45">
-      <c r="A6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>2347</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.9" x14ac:dyDescent="0.45">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>2348</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.9" x14ac:dyDescent="0.45">
-      <c r="A8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>2349</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.9" x14ac:dyDescent="0.45">
-      <c r="A9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>2350</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.9" x14ac:dyDescent="0.45">
-      <c r="A10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>2351</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.9" x14ac:dyDescent="0.45">
-      <c r="A11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>2352</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.9" x14ac:dyDescent="0.45">
-      <c r="A12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>2353</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.9" x14ac:dyDescent="0.45">
-      <c r="A13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>2354</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.9" x14ac:dyDescent="0.45">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:D1"/>
-  <conditionalFormatting sqref="D2:D13">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://codes.iarc.fr/code/2326"/>
-    <hyperlink ref="B3" r:id="rId2" display="http://codes.iarc.fr/code/2565"/>
-    <hyperlink ref="B4" r:id="rId3" display="http://codes.iarc.fr/code/2724"/>
-    <hyperlink ref="B5" r:id="rId4" display="http://codes.iarc.fr/code/2759"/>
-    <hyperlink ref="B6" r:id="rId5" display="http://codes.iarc.fr/code/2768"/>
-    <hyperlink ref="B7" r:id="rId6" display="http://codes.iarc.fr/code/2771"/>
-    <hyperlink ref="B8" r:id="rId7" display="http://codes.iarc.fr/code/3068"/>
-    <hyperlink ref="B9" r:id="rId8" display="http://codes.iarc.fr/code/3200"/>
-    <hyperlink ref="B10" r:id="rId9" display="http://codes.iarc.fr/code/3591"/>
-    <hyperlink ref="B11" r:id="rId10" display="http://codes.iarc.fr/code/3695"/>
-    <hyperlink ref="B12" r:id="rId11" display="http://codes.iarc.fr/code/3759"/>
-    <hyperlink ref="B13" r:id="rId12" display="http://codes.iarc.fr/code/3806"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>